<commit_message>
Arreglat Cronometre a FiveDigits
</commit_message>
<xml_diff>
--- a/TFG/res/pacientData/1234/Resultats.xlsx
+++ b/TFG/res/pacientData/1234/Resultats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="507">
   <si>
     <t>Pacient</t>
   </si>
@@ -38,16 +38,16 @@
     <t>Estat civil</t>
   </si>
   <si>
-    <t>ProfessiÃ³</t>
+    <t>Professió</t>
   </si>
   <si>
     <t>Categoria professional</t>
   </si>
   <si>
-    <t>SituaciÃ³ laboral</t>
-  </si>
-  <si>
-    <t>Nivell socioeconÃ²mic</t>
+    <t>Situació laboral</t>
+  </si>
+  <si>
+    <t>Nivell socioeconòmic</t>
   </si>
   <si>
     <t>Fumador/a actualment</t>
@@ -65,7 +65,7 @@
     <t>Consum d'alcohol actual</t>
   </si>
   <si>
-    <t>NÃºm. i tipus de begudes alcohÃ²liques/dia</t>
+    <t>Núm. i tipus de begudes alcohòliques/dia</t>
   </si>
   <si>
     <t>UBE/dia</t>
@@ -77,10 +77,10 @@
     <t>Edat inici alcohol</t>
   </si>
   <si>
-    <t>Malalties crÃ²niqus concomitants</t>
-  </si>
-  <si>
-    <t>Temps en tractament no farmacolÃ²gic</t>
+    <t>Malalties cròniqus concomitants</t>
+  </si>
+  <si>
+    <t>Temps en tractament no farmacològic</t>
   </si>
   <si>
     <t>Malaltia d'Alzheimer</t>
@@ -92,7 +92,7 @@
     <t>Sindrome de Down</t>
   </si>
   <si>
-    <t>Altres demÃ¨ncies</t>
+    <t>Altres demències</t>
   </si>
   <si>
     <t>Antecedents del pare</t>
@@ -104,7 +104,7 @@
     <t>Altres familiars</t>
   </si>
   <si>
-    <t>CafÃ¨ i te</t>
+    <t>Cafè i te</t>
   </si>
   <si>
     <t>Tabac</t>
@@ -116,34 +116,34 @@
     <t>Cannabis</t>
   </si>
   <si>
-    <t>Feina i tÃ²xics laborals</t>
+    <t>Feina i tòxics laborals</t>
   </si>
   <si>
     <t>Altres antecedents personals</t>
   </si>
   <si>
-    <t>HipertensiÃ³</t>
+    <t>Hipertensió</t>
   </si>
   <si>
     <t>Data</t>
   </si>
   <si>
-    <t>InsuficiÃ¨ncia cardÃ­aca</t>
+    <t>Insuficiència cardíaca</t>
   </si>
   <si>
     <t>Infart de miocardi</t>
   </si>
   <si>
-    <t>Cardiopatia isquÃ¨mica</t>
+    <t>Cardiopatia isquèmica</t>
   </si>
   <si>
     <t>Arritmia</t>
   </si>
   <si>
-    <t>Malaltia vascular perifÃ¨rica arterial</t>
-  </si>
-  <si>
-    <t>DiabÃ¨tis</t>
+    <t>Malaltia vascular perifèrica arterial</t>
+  </si>
+  <si>
+    <t>Diabètis</t>
   </si>
   <si>
     <t>Obesitat</t>
@@ -167,7 +167,7 @@
     <t>Hepatopatia</t>
   </si>
   <si>
-    <t>DepressiÃ³</t>
+    <t>Depressió</t>
   </si>
   <si>
     <t>Ansietat</t>
@@ -176,10 +176,10 @@
     <t>Psicosis</t>
   </si>
   <si>
-    <t>AbÃºs d'alcohol</t>
-  </si>
-  <si>
-    <t>AbÃºs de drogues</t>
+    <t>Abús d'alcohol</t>
+  </si>
+  <si>
+    <t>Abús de drogues</t>
   </si>
   <si>
     <t>AVC establert</t>
@@ -188,13 +188,13 @@
     <t>AVC transitori</t>
   </si>
   <si>
-    <t>EpilÃ¨psia</t>
+    <t>Epilèpsia</t>
   </si>
   <si>
     <t>Trauma craneal greu</t>
   </si>
   <si>
-    <t>Esclerosis mÃºltiple</t>
+    <t>Esclerosis múltiple</t>
   </si>
   <si>
     <t>Cefalea</t>
@@ -206,13 +206,13 @@
     <t>EPOC</t>
   </si>
   <si>
-    <t>AnÃ¨mia</t>
+    <t>Anèmia</t>
   </si>
   <si>
     <t>Leucosis</t>
   </si>
   <si>
-    <t>AlÂ·lÃ¨rgia</t>
+    <t>Al·lèrgia</t>
   </si>
   <si>
     <t>Glaucoma</t>
@@ -242,10 +242,10 @@
     <t>Maligne</t>
   </si>
   <si>
-    <t>AnsiolÃ­tics i sedants</t>
-  </si>
-  <si>
-    <t>HipnÃ²tics</t>
+    <t>Ansiolítics i sedants</t>
+  </si>
+  <si>
+    <t>Hipnòtics</t>
   </si>
   <si>
     <t>Antidepresius</t>
@@ -254,7 +254,7 @@
     <t>Animaniacs</t>
   </si>
   <si>
-    <t>AnipsicÃ²tics/NeurolÃ¨ptics</t>
+    <t>Anipsicòtics/Neurolèptics</t>
   </si>
   <si>
     <t>Animigranyosos</t>
@@ -263,16 +263,16 @@
     <t>Opioides</t>
   </si>
   <si>
-    <t>AntiepilÃ¨ptics/Anticonvulsivants</t>
+    <t>Antiepilèptics/Anticonvulsivants</t>
   </si>
   <si>
     <t>Antiparkinsonians</t>
   </si>
   <si>
-    <t>FÃ rmacs i mÃºscul estriat</t>
-  </si>
-  <si>
-    <t>Vasodilatadors cerebrals i nootrÃ²pics</t>
+    <t>Fàrmacs i múscul estriat</t>
+  </si>
+  <si>
+    <t>Vasodilatadors cerebrals i nootròpics</t>
   </si>
   <si>
     <t>Alzheimer: inhibidors de la Ac-esterasa</t>
@@ -284,85 +284,85 @@
     <t>Psicoestimulants</t>
   </si>
   <si>
-    <t>SubstÃ ncies d'abÃºs</t>
-  </si>
-  <si>
-    <t>DeshabituaciÃ³ de substÃ ncies d'abÃºs</t>
-  </si>
-  <si>
-    <t>AntiÃ cids/protectors gÃ strics</t>
-  </si>
-  <si>
-    <t>AntidiabÃ¨tics</t>
-  </si>
-  <si>
-    <t>AntitrombÃ²tics/Anticoagulants</t>
+    <t>Substàncies d'abús</t>
+  </si>
+  <si>
+    <t>Deshabituació de substàncies d'abús</t>
+  </si>
+  <si>
+    <t>Antiàcids/protectors gàstrics</t>
+  </si>
+  <si>
+    <t>Antidiabètics</t>
+  </si>
+  <si>
+    <t>Antitrombòtics/Anticoagulants</t>
   </si>
   <si>
     <t>Antiagregants</t>
   </si>
   <si>
-    <t>CardiotÃ²nics/Antiarritmics</t>
+    <t>Cardiotònics/Antiarritmics</t>
   </si>
   <si>
     <t>Antihipertenius</t>
   </si>
   <si>
-    <t>DiurÃ¨tics</t>
+    <t>Diurètics</t>
   </si>
   <si>
     <t>Hipolipemiants</t>
   </si>
   <si>
-    <t>DermatolÃ²gics</t>
+    <t>Dermatològics</t>
   </si>
   <si>
     <t>Hormones sexuals</t>
   </si>
   <si>
-    <t>UrolÃ²gics</t>
-  </si>
-  <si>
-    <t>Corticosteroides sintÃ¨tics</t>
+    <t>Urològics</t>
+  </si>
+  <si>
+    <t>Corticosteroides sintètics</t>
   </si>
   <si>
     <t>Terapia tiroidea</t>
   </si>
   <si>
-    <t>AntineapÃ stics/Immunomoduladors</t>
-  </si>
-  <si>
-    <t>Antiinflamatoris/AntirreumÃ tics</t>
-  </si>
-  <si>
-    <t>AnalgÃ¨sics/AntipirÃ¨tics</t>
+    <t>Antineapàstics/Immunomoduladors</t>
+  </si>
+  <si>
+    <t>Antiinflamatoris/Antirreumàtics</t>
+  </si>
+  <si>
+    <t>Analgèsics/Antipirètics</t>
   </si>
   <si>
     <t>Broncodilatadors</t>
   </si>
   <si>
-    <t>OftalmolÃ²gics</t>
+    <t>Oftalmològics</t>
   </si>
   <si>
     <t>ECG: codi resultat</t>
   </si>
   <si>
-    <t>DescripciÃ³</t>
-  </si>
-  <si>
-    <t>AnalÃ­tica de sang: codi resultat</t>
-  </si>
-  <si>
-    <t>AnalÃ­tica d'orina: codi resultat</t>
-  </si>
-  <si>
-    <t>AnalÃ­tica de LCR: codi resultat</t>
-  </si>
-  <si>
-    <t>GenÃ¨tica: codi resultat</t>
-  </si>
-  <si>
-    <t>RX de tÃ²rax: codi resultat</t>
+    <t>Descripció</t>
+  </si>
+  <si>
+    <t>Analítica de sang: codi resultat</t>
+  </si>
+  <si>
+    <t>Analítica d'orina: codi resultat</t>
+  </si>
+  <si>
+    <t>Analítica de LCR: codi resultat</t>
+  </si>
+  <si>
+    <t>Genètica: codi resultat</t>
+  </si>
+  <si>
+    <t>RX de tòrax: codi resultat</t>
   </si>
   <si>
     <t>EEG: codi resultat</t>
@@ -377,7 +377,7 @@
     <t>N-TMS: codi resultat</t>
   </si>
   <si>
-    <t>Anatomia patolÃ²gica: codi resultat</t>
+    <t>Anatomia patològica: codi resultat</t>
   </si>
   <si>
     <t>TC: codi resultat</t>
@@ -707,19 +707,19 @@
     <t>FD - Eleccio Errors PC_T1</t>
   </si>
   <si>
-    <t>Five Digits - AlternanÃ§a Temps_T1</t>
-  </si>
-  <si>
-    <t>FD - AlternanÃ§a Temps PC_T1</t>
-  </si>
-  <si>
-    <t>FD - AlternanÃ§a Errors_T1</t>
-  </si>
-  <si>
-    <t>FD - AlternanÃ§a Errors PC_T1</t>
-  </si>
-  <si>
-    <t>Five Digits - InhibiciÃ³ PC_T1</t>
+    <t>Five Digits - Alternança Temps_T1</t>
+  </si>
+  <si>
+    <t>FD - Alternança Temps PC_T1</t>
+  </si>
+  <si>
+    <t>FD - Alternança Errors_T1</t>
+  </si>
+  <si>
+    <t>FD - Alternança Errors PC_T1</t>
+  </si>
+  <si>
+    <t>Five Digits - Inhibició PC_T1</t>
   </si>
   <si>
     <t>Five Digits - Flexibilitat PC_T1</t>
@@ -743,7 +743,7 @@
     <t>UPSA Comunicacio_T1</t>
   </si>
   <si>
-    <t>UPSA ComprensiÃ³_T1</t>
+    <t>UPSA Comprensió_T1</t>
   </si>
   <si>
     <t>UPSA total_T1</t>
@@ -1064,19 +1064,19 @@
     <t>FD - Eleccio Errors PC_T2</t>
   </si>
   <si>
-    <t>Five Digits - AlternanÃ§a Temps_T2</t>
-  </si>
-  <si>
-    <t>FD - AlternanÃ§a Temps PC_T2</t>
-  </si>
-  <si>
-    <t>FD - AlternanÃ§a Errors_T2</t>
-  </si>
-  <si>
-    <t>FD - AlternanÃ§a Errors PC_T2</t>
-  </si>
-  <si>
-    <t>Five Digits - InhibiciÃ³ PC_T2</t>
+    <t>Five Digits - Alternança Temps_T2</t>
+  </si>
+  <si>
+    <t>FD - Alternança Temps PC_T2</t>
+  </si>
+  <si>
+    <t>FD - Alternança Errors_T2</t>
+  </si>
+  <si>
+    <t>FD - Alternança Errors PC_T2</t>
+  </si>
+  <si>
+    <t>Five Digits - Inhibició PC_T2</t>
   </si>
   <si>
     <t>Five Digits - Flexibilitat PC_T2</t>
@@ -1100,7 +1100,7 @@
     <t>UPSA Comunicacio_T2</t>
   </si>
   <si>
-    <t>UPSA ComprensiÃ³_T2</t>
+    <t>UPSA Comprensió_T2</t>
   </si>
   <si>
     <t>UPSA total_T2</t>
@@ -1421,19 +1421,19 @@
     <t>FD - Eleccio Errors PC_T3</t>
   </si>
   <si>
-    <t>Five Digits - AlternanÃ§a Temps_T3</t>
-  </si>
-  <si>
-    <t>FD - AlternanÃ§a Temps PC_T3</t>
-  </si>
-  <si>
-    <t>FD - AlternanÃ§a Errors_T3</t>
-  </si>
-  <si>
-    <t>FD - AlternanÃ§a Errors PC_T3</t>
-  </si>
-  <si>
-    <t>Five Digits - InhibiciÃ³ PC_T3</t>
+    <t>Five Digits - Alternança Temps_T3</t>
+  </si>
+  <si>
+    <t>FD - Alternança Temps PC_T3</t>
+  </si>
+  <si>
+    <t>FD - Alternança Errors_T3</t>
+  </si>
+  <si>
+    <t>FD - Alternança Errors PC_T3</t>
+  </si>
+  <si>
+    <t>Five Digits - Inhibició PC_T3</t>
   </si>
   <si>
     <t>Five Digits - Flexibilitat PC_T3</t>
@@ -1457,7 +1457,7 @@
     <t>UPSA Comunicacio_T3</t>
   </si>
   <si>
-    <t>UPSA ComprensiÃ³_T3</t>
+    <t>UPSA Comprensió_T3</t>
   </si>
   <si>
     <t>UPSA total_T3</t>
@@ -1499,7 +1499,7 @@
     <t>Home</t>
   </si>
   <si>
-    <t>NomÃ©s castellÃ </t>
+    <t>Només castellà</t>
   </si>
   <si>
     <t>11/02/1955</t>
@@ -1518,6 +1518,21 @@
   </si>
   <si>
     <t>Jubilat</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>00:04.83</t>
+  </si>
+  <si>
+    <t>00:04.67</t>
+  </si>
+  <si>
+    <t>00:02.87</t>
+  </si>
+  <si>
+    <t>adfg</t>
   </si>
 </sst>
 </file>
@@ -3362,6 +3377,924 @@
       <c r="J2" t="s">
         <v>501</v>
       </c>
+      <c r="K2" t="s">
+        <v>135</v>
+      </c>
+      <c r="L2" t="s">
+        <v>135</v>
+      </c>
+      <c r="M2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N2" t="s">
+        <v>135</v>
+      </c>
+      <c r="O2" t="s">
+        <v>135</v>
+      </c>
+      <c r="P2" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>135</v>
+      </c>
+      <c r="R2" t="s">
+        <v>135</v>
+      </c>
+      <c r="S2" t="s">
+        <v>135</v>
+      </c>
+      <c r="T2" t="s">
+        <v>135</v>
+      </c>
+      <c r="U2" t="s">
+        <v>135</v>
+      </c>
+      <c r="V2" t="s">
+        <v>135</v>
+      </c>
+      <c r="W2" t="s">
+        <v>135</v>
+      </c>
+      <c r="X2" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>135</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>135</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>135</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>135</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="ER2" t="s">
+        <v>135</v>
+      </c>
+      <c r="ES2" t="s">
+        <v>135</v>
+      </c>
+      <c r="ET2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EU2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EV2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EW2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EX2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EY2" t="s">
+        <v>135</v>
+      </c>
+      <c r="EZ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FA2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FB2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FC2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FD2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FE2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FF2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FG2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FH2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FI2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FJ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FK2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FL2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FM2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FN2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FO2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FP2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FQ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FR2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FS2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FT2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FU2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FV2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FW2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FX2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FY2" t="s">
+        <v>135</v>
+      </c>
+      <c r="FZ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GA2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GB2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GC2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GD2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GE2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GF2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GG2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GH2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GI2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GJ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GK2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GL2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GM2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GN2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GO2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GP2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GQ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GR2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GS2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GT2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GU2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GV2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GW2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GX2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GY2" t="s">
+        <v>135</v>
+      </c>
+      <c r="GZ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HA2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HB2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HC2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HD2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HE2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HF2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HG2" t="s">
+        <v>502</v>
+      </c>
+      <c r="HH2" t="s">
+        <v>502</v>
+      </c>
+      <c r="HI2" t="s">
+        <v>502</v>
+      </c>
+      <c r="HJ2" t="s">
+        <v>502</v>
+      </c>
+      <c r="HK2" t="s">
+        <v>502</v>
+      </c>
+      <c r="HL2" t="s">
+        <v>502</v>
+      </c>
+      <c r="HM2" t="s">
+        <v>502</v>
+      </c>
+      <c r="HN2" t="s">
+        <v>502</v>
+      </c>
+      <c r="HO2" t="s">
+        <v>502</v>
+      </c>
+      <c r="HP2" t="s">
+        <v>502</v>
+      </c>
+      <c r="HQ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HR2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HS2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HT2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HU2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HV2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HW2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HX2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HY2" t="s">
+        <v>135</v>
+      </c>
+      <c r="HZ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IA2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IB2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IC2" t="s">
+        <v>135</v>
+      </c>
+      <c r="ID2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IE2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IF2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IG2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IH2" t="s">
+        <v>135</v>
+      </c>
+      <c r="II2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IJ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IK2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IL2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IM2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IN2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IO2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IP2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IQ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IR2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IS2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IT2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IU2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IV2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IW2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IX2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IY2" t="s">
+        <v>135</v>
+      </c>
+      <c r="IZ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JA2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JB2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JC2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JD2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JE2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JF2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JG2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JH2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JI2" t="s">
+        <v>502</v>
+      </c>
+      <c r="JJ2" t="s">
+        <v>502</v>
+      </c>
+      <c r="JK2" t="s">
+        <v>502</v>
+      </c>
+      <c r="JL2" t="s">
+        <v>502</v>
+      </c>
+      <c r="JM2" t="s">
+        <v>502</v>
+      </c>
+      <c r="JN2" t="s">
+        <v>502</v>
+      </c>
+      <c r="JO2" t="s">
+        <v>502</v>
+      </c>
+      <c r="JP2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JQ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JR2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JS2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JT2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JU2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JV2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JW2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JX2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JY2" t="s">
+        <v>135</v>
+      </c>
+      <c r="JZ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KA2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KB2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KC2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KD2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KE2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KF2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KG2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KH2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KI2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KJ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KK2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KL2" t="s">
+        <v>503</v>
+      </c>
+      <c r="KM2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KN2" t="s">
+        <v>502</v>
+      </c>
+      <c r="KO2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KP2" t="s">
+        <v>504</v>
+      </c>
+      <c r="KQ2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KR2" t="s">
+        <v>502</v>
+      </c>
+      <c r="KS2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KT2" t="s">
+        <v>503</v>
+      </c>
+      <c r="KU2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KV2" t="s">
+        <v>502</v>
+      </c>
+      <c r="KW2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KX2" t="s">
+        <v>505</v>
+      </c>
+      <c r="KY2" t="s">
+        <v>135</v>
+      </c>
+      <c r="KZ2" t="s">
+        <v>502</v>
+      </c>
+      <c r="LA2" t="s">
+        <v>135</v>
+      </c>
+      <c r="LB2" t="s">
+        <v>135</v>
+      </c>
+      <c r="LC2" t="s">
+        <v>135</v>
+      </c>
+      <c r="LD2" t="s">
+        <v>506</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Moltes millores i guardar resultats
</commit_message>
<xml_diff>
--- a/TFG/res/pacientData/1234/Resultats.xlsx
+++ b/TFG/res/pacientData/1234/Resultats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="582">
   <si>
     <t>Pacient</t>
   </si>
@@ -38,16 +38,16 @@
     <t>Estat civil</t>
   </si>
   <si>
-    <t>Professió</t>
+    <t>Professio</t>
   </si>
   <si>
     <t>Categoria professional</t>
   </si>
   <si>
-    <t>Situació laboral</t>
-  </si>
-  <si>
-    <t>Nivell socioeconòmic</t>
+    <t>Situacio laboral</t>
+  </si>
+  <si>
+    <t>Nivell socioeconomic</t>
   </si>
   <si>
     <t>Fumador/a actualment</t>
@@ -65,7 +65,7 @@
     <t>Consum d'alcohol actual</t>
   </si>
   <si>
-    <t>Núm. i tipus de begudes alcohòliques/dia</t>
+    <t>Num. i tipus de begudes alcoholiques/dia</t>
   </si>
   <si>
     <t>UBE/dia</t>
@@ -77,10 +77,10 @@
     <t>Edat inici alcohol</t>
   </si>
   <si>
-    <t>Malalties cròniqus concomitants</t>
-  </si>
-  <si>
-    <t>Temps en tractament no farmacològic</t>
+    <t>Malalties croniqus concomitants</t>
+  </si>
+  <si>
+    <t>Temps en tractament no farmacologic</t>
   </si>
   <si>
     <t>Malaltia d'Alzheimer</t>
@@ -92,7 +92,7 @@
     <t>Sindrome de Down</t>
   </si>
   <si>
-    <t>Altres demències</t>
+    <t>Altres demencies</t>
   </si>
   <si>
     <t>Antecedents del pare</t>
@@ -104,7 +104,7 @@
     <t>Altres familiars</t>
   </si>
   <si>
-    <t>Cafè i te</t>
+    <t>Cafe i te</t>
   </si>
   <si>
     <t>Tabac</t>
@@ -116,34 +116,34 @@
     <t>Cannabis</t>
   </si>
   <si>
-    <t>Feina i tòxics laborals</t>
+    <t>Feina i toxics laborals</t>
   </si>
   <si>
     <t>Altres antecedents personals</t>
   </si>
   <si>
-    <t>Hipertensió</t>
+    <t>Hipertensio</t>
   </si>
   <si>
     <t>Data</t>
   </si>
   <si>
-    <t>Insuficiència cardíaca</t>
+    <t>Insuficiencia cardiaca</t>
   </si>
   <si>
     <t>Infart de miocardi</t>
   </si>
   <si>
-    <t>Cardiopatia isquèmica</t>
+    <t>Cardiopatia isquemica</t>
   </si>
   <si>
     <t>Arritmia</t>
   </si>
   <si>
-    <t>Malaltia vascular perifèrica arterial</t>
-  </si>
-  <si>
-    <t>Diabètis</t>
+    <t>Malaltia vascular periferica arterial</t>
+  </si>
+  <si>
+    <t>Diabetis</t>
   </si>
   <si>
     <t>Obesitat</t>
@@ -167,7 +167,7 @@
     <t>Hepatopatia</t>
   </si>
   <si>
-    <t>Depressió</t>
+    <t>Depressio</t>
   </si>
   <si>
     <t>Ansietat</t>
@@ -176,10 +176,10 @@
     <t>Psicosis</t>
   </si>
   <si>
-    <t>Abús d'alcohol</t>
-  </si>
-  <si>
-    <t>Abús de drogues</t>
+    <t>Abus d'alcohol</t>
+  </si>
+  <si>
+    <t>Abus de drogues</t>
   </si>
   <si>
     <t>AVC establert</t>
@@ -188,13 +188,13 @@
     <t>AVC transitori</t>
   </si>
   <si>
-    <t>Epilèpsia</t>
+    <t>Epilepsia</t>
   </si>
   <si>
     <t>Trauma craneal greu</t>
   </si>
   <si>
-    <t>Esclerosis múltiple</t>
+    <t>Esclerosis multiple</t>
   </si>
   <si>
     <t>Cefalea</t>
@@ -206,13 +206,13 @@
     <t>EPOC</t>
   </si>
   <si>
-    <t>Anèmia</t>
+    <t>Anemia</t>
   </si>
   <si>
     <t>Leucosis</t>
   </si>
   <si>
-    <t>Al·lèrgia</t>
+    <t>Al.lergia</t>
   </si>
   <si>
     <t>Glaucoma</t>
@@ -242,10 +242,10 @@
     <t>Maligne</t>
   </si>
   <si>
-    <t>Ansiolítics i sedants</t>
-  </si>
-  <si>
-    <t>Hipnòtics</t>
+    <t>Ansiolitics i sedants</t>
+  </si>
+  <si>
+    <t>Hipnotics</t>
   </si>
   <si>
     <t>Antidepresius</t>
@@ -254,7 +254,7 @@
     <t>Animaniacs</t>
   </si>
   <si>
-    <t>Anipsicòtics/Neurolèptics</t>
+    <t>Anipsicotics/Neuroleptics</t>
   </si>
   <si>
     <t>Animigranyosos</t>
@@ -263,16 +263,16 @@
     <t>Opioides</t>
   </si>
   <si>
-    <t>Antiepilèptics/Anticonvulsivants</t>
+    <t>Antiepileptics/Anticonvulsivants</t>
   </si>
   <si>
     <t>Antiparkinsonians</t>
   </si>
   <si>
-    <t>Fàrmacs i múscul estriat</t>
-  </si>
-  <si>
-    <t>Vasodilatadors cerebrals i nootròpics</t>
+    <t>Farmacs i muscul estriat</t>
+  </si>
+  <si>
+    <t>Vasodilatadors cerebrals i nootropics</t>
   </si>
   <si>
     <t>Alzheimer: inhibidors de la Ac-esterasa</t>
@@ -284,85 +284,85 @@
     <t>Psicoestimulants</t>
   </si>
   <si>
-    <t>Substàncies d'abús</t>
-  </si>
-  <si>
-    <t>Deshabituació de substàncies d'abús</t>
-  </si>
-  <si>
-    <t>Antiàcids/protectors gàstrics</t>
-  </si>
-  <si>
-    <t>Antidiabètics</t>
-  </si>
-  <si>
-    <t>Antitrombòtics/Anticoagulants</t>
+    <t>Substancies d'abus</t>
+  </si>
+  <si>
+    <t>Deshabituacio de substancies d'abus</t>
+  </si>
+  <si>
+    <t>Antiacids/protectors gastrics</t>
+  </si>
+  <si>
+    <t>Antidiabetics</t>
+  </si>
+  <si>
+    <t>Antitrombotics/Anticoagulants</t>
   </si>
   <si>
     <t>Antiagregants</t>
   </si>
   <si>
-    <t>Cardiotònics/Antiarritmics</t>
+    <t>Cardiotonics/Antiarritmics</t>
   </si>
   <si>
     <t>Antihipertenius</t>
   </si>
   <si>
-    <t>Diurètics</t>
+    <t>Diuretics</t>
   </si>
   <si>
     <t>Hipolipemiants</t>
   </si>
   <si>
-    <t>Dermatològics</t>
+    <t>Dermatologics</t>
   </si>
   <si>
     <t>Hormones sexuals</t>
   </si>
   <si>
-    <t>Urològics</t>
-  </si>
-  <si>
-    <t>Corticosteroides sintètics</t>
+    <t>Urologics</t>
+  </si>
+  <si>
+    <t>Corticosteroides sintetics</t>
   </si>
   <si>
     <t>Terapia tiroidea</t>
   </si>
   <si>
-    <t>Antineapàstics/Immunomoduladors</t>
-  </si>
-  <si>
-    <t>Antiinflamatoris/Antirreumàtics</t>
-  </si>
-  <si>
-    <t>Analgèsics/Antipirètics</t>
+    <t>Antineapastics/Immunomoduladors</t>
+  </si>
+  <si>
+    <t>Antiinflamatoris/Antirreumatics</t>
+  </si>
+  <si>
+    <t>Analgesics/Antipiretics</t>
   </si>
   <si>
     <t>Broncodilatadors</t>
   </si>
   <si>
-    <t>Oftalmològics</t>
+    <t>Oftalmologics</t>
   </si>
   <si>
     <t>ECG: codi resultat</t>
   </si>
   <si>
-    <t>Descripció</t>
-  </si>
-  <si>
-    <t>Analítica de sang: codi resultat</t>
-  </si>
-  <si>
-    <t>Analítica d'orina: codi resultat</t>
-  </si>
-  <si>
-    <t>Analítica de LCR: codi resultat</t>
-  </si>
-  <si>
-    <t>Genètica: codi resultat</t>
-  </si>
-  <si>
-    <t>RX de tòrax: codi resultat</t>
+    <t>Descripcio</t>
+  </si>
+  <si>
+    <t>Analitica de sang: codi resultat</t>
+  </si>
+  <si>
+    <t>Analitica d'orina: codi resultat</t>
+  </si>
+  <si>
+    <t>Analitica de LCR: codi resultat</t>
+  </si>
+  <si>
+    <t>Genetica: codi resultat</t>
+  </si>
+  <si>
+    <t>RX de torax: codi resultat</t>
   </si>
   <si>
     <t>EEG: codi resultat</t>
@@ -377,7 +377,7 @@
     <t>N-TMS: codi resultat</t>
   </si>
   <si>
-    <t>Anatomia patològica: codi resultat</t>
+    <t>Anatomia patologica: codi resultat</t>
   </si>
   <si>
     <t>TC: codi resultat</t>
@@ -719,7 +719,7 @@
     <t>FD - Alternança Errors PC_T1</t>
   </si>
   <si>
-    <t>Five Digits - Inhibició PC_T1</t>
+    <t>Five Digits - Inhibicio PC_T1</t>
   </si>
   <si>
     <t>Five Digits - Flexibilitat PC_T1</t>
@@ -743,7 +743,7 @@
     <t>UPSA Comunicacio_T1</t>
   </si>
   <si>
-    <t>UPSA Comprensió_T1</t>
+    <t>UPSA Comprensio_T1</t>
   </si>
   <si>
     <t>UPSA total_T1</t>
@@ -1076,7 +1076,7 @@
     <t>FD - Alternança Errors PC_T2</t>
   </si>
   <si>
-    <t>Five Digits - Inhibició PC_T2</t>
+    <t>Five Digits - Inhibicio PC_T2</t>
   </si>
   <si>
     <t>Five Digits - Flexibilitat PC_T2</t>
@@ -1100,7 +1100,7 @@
     <t>UPSA Comunicacio_T2</t>
   </si>
   <si>
-    <t>UPSA Comprensió_T2</t>
+    <t>UPSA Comprensio_T2</t>
   </si>
   <si>
     <t>UPSA total_T2</t>
@@ -1433,7 +1433,7 @@
     <t>FD - Alternança Errors PC_T3</t>
   </si>
   <si>
-    <t>Five Digits - Inhibició PC_T3</t>
+    <t>Five Digits - Inhibicio PC_T3</t>
   </si>
   <si>
     <t>Five Digits - Flexibilitat PC_T3</t>
@@ -1457,7 +1457,7 @@
     <t>UPSA Comunicacio_T3</t>
   </si>
   <si>
-    <t>UPSA Comprensió_T3</t>
+    <t>UPSA Comprensio_T3</t>
   </si>
   <si>
     <t>UPSA total_T3</t>
@@ -1505,10 +1505,7 @@
     <t>11/02/1955</t>
   </si>
   <si>
-    <t>Sense estudis</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sap llegir i escriure</t>
+    <t>Sense estudis-sap llegir i escriure</t>
   </si>
   <si>
     <t>10</t>
@@ -1518,6 +1515,234 @@
   </si>
   <si>
     <t>Jubilat</t>
+  </si>
+  <si>
+    <t>Tècnic professional de nivell mig</t>
+  </si>
+  <si>
+    <t>Atur</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Ara no, anteriorment sí (fa més de 12 mesos que no en fa)</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>erqtt</t>
+  </si>
+  <si>
+    <t>ertwert</t>
+  </si>
+  <si>
+    <t>efgf</t>
+  </si>
+  <si>
+    <t>dfgdfg</t>
+  </si>
+  <si>
+    <t>20/04/2017</t>
+  </si>
+  <si>
+    <t>11/04/2017</t>
+  </si>
+  <si>
+    <t>14/04/2017</t>
+  </si>
+  <si>
+    <t>19/04/2017</t>
+  </si>
+  <si>
+    <t>07/04/2017</t>
+  </si>
+  <si>
+    <t>22/04/2017</t>
+  </si>
+  <si>
+    <t>21/04/2017</t>
+  </si>
+  <si>
+    <t>15/04/2017</t>
+  </si>
+  <si>
+    <t>24/04/2017</t>
+  </si>
+  <si>
+    <t>09/04/2017</t>
+  </si>
+  <si>
+    <t>25/04/2017</t>
+  </si>
+  <si>
+    <t>12/04/2017</t>
+  </si>
+  <si>
+    <t>werqer</t>
+  </si>
+  <si>
+    <t>thtyj</t>
+  </si>
+  <si>
+    <t>hjkl</t>
+  </si>
+  <si>
+    <t>iúp</t>
+  </si>
+  <si>
+    <t>ryuey</t>
+  </si>
+  <si>
+    <t>tretrhw</t>
+  </si>
+  <si>
+    <t>wrt</t>
+  </si>
+  <si>
+    <t>rthetyj</t>
+  </si>
+  <si>
+    <t>etykryuktu</t>
+  </si>
+  <si>
+    <t>tuiltui</t>
+  </si>
+  <si>
+    <t>ruyir</t>
+  </si>
+  <si>
+    <t>etywtu</t>
+  </si>
+  <si>
+    <t>wrtywrtw</t>
+  </si>
+  <si>
+    <t>wrthwrthe</t>
+  </si>
+  <si>
+    <t>eyuiryui</t>
+  </si>
+  <si>
+    <t>ruotuy</t>
+  </si>
+  <si>
+    <t>ertghwtgh</t>
+  </si>
+  <si>
+    <t>wertywrth</t>
+  </si>
+  <si>
+    <t>fghetyj</t>
+  </si>
+  <si>
+    <t>rfghrgn</t>
+  </si>
+  <si>
+    <t>wrthywrty</t>
+  </si>
+  <si>
+    <t>wrtywrty</t>
+  </si>
+  <si>
+    <t>wrtywrtywrtywrty</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>dfgafg</t>
+  </si>
+  <si>
+    <t>27/04/2017</t>
+  </si>
+  <si>
+    <t>adfgadfg</t>
+  </si>
+  <si>
+    <t>Anormal NCS</t>
+  </si>
+  <si>
+    <t>No realitzat</t>
+  </si>
+  <si>
+    <t>dfgadfg</t>
+  </si>
+  <si>
+    <t>dfhafghg</t>
+  </si>
+  <si>
+    <t>05/04/2017</t>
+  </si>
+  <si>
+    <t>adfgafg</t>
+  </si>
+  <si>
+    <t>06/04/2017</t>
+  </si>
+  <si>
+    <t>adfgadgf</t>
+  </si>
+  <si>
+    <t>Anormal CS</t>
+  </si>
+  <si>
+    <t>adfafg</t>
+  </si>
+  <si>
+    <t>adfgadfga</t>
+  </si>
+  <si>
+    <t>adfgadfgag</t>
+  </si>
+  <si>
+    <t>3,0 (Deteriorament greu)</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>22</t>
   </si>
   <si>
     <t>0</t>
@@ -3378,526 +3603,526 @@
         <v>501</v>
       </c>
       <c r="K2" t="s">
-        <v>135</v>
+        <v>502</v>
       </c>
       <c r="L2" t="s">
-        <v>135</v>
+        <v>503</v>
       </c>
       <c r="M2" t="s">
-        <v>135</v>
+        <v>504</v>
       </c>
       <c r="N2" t="s">
-        <v>135</v>
+        <v>505</v>
       </c>
       <c r="O2" t="s">
-        <v>135</v>
+        <v>506</v>
       </c>
       <c r="P2" t="s">
-        <v>135</v>
+        <v>507</v>
       </c>
       <c r="Q2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="R2" t="s">
-        <v>135</v>
+        <v>503</v>
       </c>
       <c r="S2" t="s">
-        <v>135</v>
+        <v>509</v>
       </c>
       <c r="T2" t="s">
-        <v>135</v>
+        <v>510</v>
       </c>
       <c r="U2" t="s">
-        <v>135</v>
+        <v>511</v>
       </c>
       <c r="V2" t="s">
-        <v>135</v>
+        <v>512</v>
       </c>
       <c r="W2" t="s">
-        <v>135</v>
+        <v>513</v>
       </c>
       <c r="X2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="Y2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="Z2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="AA2" t="s">
-        <v>135</v>
+        <v>493</v>
       </c>
       <c r="AB2" t="s">
-        <v>135</v>
+        <v>514</v>
       </c>
       <c r="AC2" t="s">
-        <v>135</v>
+        <v>515</v>
       </c>
       <c r="AD2" t="s">
-        <v>135</v>
+        <v>516</v>
       </c>
       <c r="AE2" t="s">
-        <v>135</v>
+        <v>505</v>
       </c>
       <c r="AF2" t="s">
-        <v>135</v>
+        <v>505</v>
       </c>
       <c r="AG2" t="s">
-        <v>135</v>
+        <v>505</v>
       </c>
       <c r="AH2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="AI2" t="s">
-        <v>135</v>
+        <v>517</v>
       </c>
       <c r="AJ2" t="s">
-        <v>135</v>
+        <v>518</v>
       </c>
       <c r="AK2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="AL2" t="s">
-        <v>135</v>
+        <v>519</v>
       </c>
       <c r="AM2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="AN2" t="s">
-        <v>135</v>
+        <v>520</v>
       </c>
       <c r="AO2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="AP2" t="s">
-        <v>135</v>
+        <v>519</v>
       </c>
       <c r="AQ2" t="s">
-        <v>135</v>
+        <v>504</v>
       </c>
       <c r="AR2" t="s">
         <v>135</v>
       </c>
       <c r="AS2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="AT2" t="s">
-        <v>135</v>
+        <v>521</v>
       </c>
       <c r="AU2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="AV2" t="s">
-        <v>135</v>
+        <v>522</v>
       </c>
       <c r="AW2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="AX2" t="s">
-        <v>135</v>
+        <v>521</v>
       </c>
       <c r="AY2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="AZ2" t="s">
-        <v>135</v>
+        <v>521</v>
       </c>
       <c r="BA2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="BB2" t="s">
-        <v>135</v>
+        <v>523</v>
       </c>
       <c r="BC2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="BD2" t="s">
-        <v>135</v>
+        <v>524</v>
       </c>
       <c r="BE2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="BF2" t="s">
-        <v>135</v>
+        <v>524</v>
       </c>
       <c r="BG2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="BH2" t="s">
-        <v>135</v>
+        <v>521</v>
       </c>
       <c r="BI2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="BJ2" t="s">
-        <v>135</v>
+        <v>519</v>
       </c>
       <c r="BK2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="BL2" t="s">
-        <v>135</v>
+        <v>525</v>
       </c>
       <c r="BM2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="BN2" t="s">
-        <v>135</v>
+        <v>521</v>
       </c>
       <c r="BO2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="BP2" t="s">
-        <v>135</v>
+        <v>521</v>
       </c>
       <c r="BQ2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="BR2" t="s">
-        <v>135</v>
+        <v>526</v>
       </c>
       <c r="BS2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="BT2" t="s">
-        <v>135</v>
+        <v>525</v>
       </c>
       <c r="BU2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="BV2" t="s">
-        <v>135</v>
+        <v>527</v>
       </c>
       <c r="BW2" t="s">
-        <v>135</v>
+        <v>504</v>
       </c>
       <c r="BX2" t="s">
         <v>135</v>
       </c>
       <c r="BY2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="BZ2" t="s">
         <v>135</v>
       </c>
       <c r="CA2" t="s">
-        <v>135</v>
+        <v>504</v>
       </c>
       <c r="CB2" t="s">
         <v>135</v>
       </c>
       <c r="CC2" t="s">
-        <v>135</v>
+        <v>504</v>
       </c>
       <c r="CD2" t="s">
         <v>135</v>
       </c>
       <c r="CE2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="CF2" t="s">
         <v>135</v>
       </c>
       <c r="CG2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="CH2" t="s">
         <v>135</v>
       </c>
       <c r="CI2" t="s">
-        <v>135</v>
+        <v>504</v>
       </c>
       <c r="CJ2" t="s">
         <v>135</v>
       </c>
       <c r="CK2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="CL2" t="s">
-        <v>135</v>
+        <v>528</v>
       </c>
       <c r="CM2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="CN2" t="s">
-        <v>135</v>
+        <v>524</v>
       </c>
       <c r="CO2" t="s">
-        <v>135</v>
+        <v>504</v>
       </c>
       <c r="CP2" t="s">
         <v>135</v>
       </c>
       <c r="CQ2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="CR2" t="s">
-        <v>135</v>
+        <v>529</v>
       </c>
       <c r="CS2" t="s">
-        <v>135</v>
+        <v>504</v>
       </c>
       <c r="CT2" t="s">
         <v>135</v>
       </c>
       <c r="CU2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="CV2" t="s">
-        <v>135</v>
+        <v>525</v>
       </c>
       <c r="CW2" t="s">
-        <v>135</v>
+        <v>504</v>
       </c>
       <c r="CX2" t="s">
         <v>135</v>
       </c>
       <c r="CY2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="CZ2" t="s">
-        <v>135</v>
+        <v>530</v>
       </c>
       <c r="DA2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="DB2" t="s">
-        <v>135</v>
+        <v>525</v>
       </c>
       <c r="DC2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="DD2" t="s">
-        <v>135</v>
+        <v>526</v>
       </c>
       <c r="DE2" t="s">
-        <v>135</v>
+        <v>508</v>
       </c>
       <c r="DF2" t="s">
-        <v>135</v>
+        <v>530</v>
       </c>
       <c r="DG2" t="s">
-        <v>135</v>
+        <v>504</v>
       </c>
       <c r="DH2" t="s">
         <v>135</v>
       </c>
       <c r="DI2" t="s">
-        <v>135</v>
+        <v>504</v>
       </c>
       <c r="DJ2" t="s">
         <v>135</v>
       </c>
       <c r="DK2" t="s">
-        <v>135</v>
+        <v>504</v>
       </c>
       <c r="DL2" t="s">
         <v>135</v>
       </c>
       <c r="DM2" t="s">
-        <v>135</v>
+        <v>531</v>
       </c>
       <c r="DN2" t="s">
-        <v>135</v>
+        <v>532</v>
       </c>
       <c r="DO2" t="s">
-        <v>135</v>
+        <v>533</v>
       </c>
       <c r="DP2" t="s">
-        <v>135</v>
+        <v>534</v>
       </c>
       <c r="DQ2" t="s">
-        <v>135</v>
+        <v>535</v>
       </c>
       <c r="DR2" t="s">
-        <v>135</v>
+        <v>536</v>
       </c>
       <c r="DS2" t="s">
-        <v>135</v>
+        <v>537</v>
       </c>
       <c r="DT2" t="s">
-        <v>135</v>
+        <v>538</v>
       </c>
       <c r="DU2" t="s">
-        <v>135</v>
+        <v>539</v>
       </c>
       <c r="DV2" t="s">
-        <v>135</v>
+        <v>540</v>
       </c>
       <c r="DW2" t="s">
-        <v>135</v>
+        <v>541</v>
       </c>
       <c r="DX2" t="s">
-        <v>135</v>
+        <v>542</v>
       </c>
       <c r="DY2" t="s">
-        <v>135</v>
+        <v>543</v>
       </c>
       <c r="DZ2" t="s">
-        <v>135</v>
+        <v>544</v>
       </c>
       <c r="EA2" t="s">
-        <v>135</v>
+        <v>545</v>
       </c>
       <c r="EB2" t="s">
-        <v>135</v>
+        <v>546</v>
       </c>
       <c r="EC2" t="s">
-        <v>135</v>
+        <v>547</v>
       </c>
       <c r="ED2" t="s">
-        <v>135</v>
+        <v>548</v>
       </c>
       <c r="EE2" t="s">
-        <v>135</v>
+        <v>549</v>
       </c>
       <c r="EF2" t="s">
-        <v>135</v>
+        <v>550</v>
       </c>
       <c r="EG2" t="s">
-        <v>135</v>
+        <v>551</v>
       </c>
       <c r="EH2" t="s">
-        <v>135</v>
+        <v>552</v>
       </c>
       <c r="EI2" t="s">
-        <v>135</v>
+        <v>553</v>
       </c>
       <c r="EJ2" t="s">
-        <v>135</v>
+        <v>505</v>
       </c>
       <c r="EK2" t="s">
-        <v>135</v>
+        <v>506</v>
       </c>
       <c r="EL2" t="s">
-        <v>135</v>
+        <v>507</v>
       </c>
       <c r="EM2" t="s">
-        <v>135</v>
+        <v>503</v>
       </c>
       <c r="EN2" t="s">
-        <v>135</v>
+        <v>510</v>
       </c>
       <c r="EO2" t="s">
-        <v>135</v>
+        <v>511</v>
       </c>
       <c r="EP2" t="s">
-        <v>135</v>
+        <v>512</v>
       </c>
       <c r="EQ2" t="s">
-        <v>135</v>
+        <v>554</v>
       </c>
       <c r="ER2" t="s">
-        <v>135</v>
+        <v>555</v>
       </c>
       <c r="ES2" t="s">
-        <v>135</v>
+        <v>498</v>
       </c>
       <c r="ET2" t="s">
-        <v>135</v>
+        <v>556</v>
       </c>
       <c r="EU2" t="s">
-        <v>135</v>
+        <v>557</v>
       </c>
       <c r="EV2" t="s">
-        <v>135</v>
+        <v>558</v>
       </c>
       <c r="EW2" t="s">
-        <v>135</v>
+        <v>559</v>
       </c>
       <c r="EX2" t="s">
-        <v>135</v>
+        <v>557</v>
       </c>
       <c r="EY2" t="s">
-        <v>135</v>
+        <v>560</v>
       </c>
       <c r="EZ2" t="s">
-        <v>135</v>
+        <v>525</v>
       </c>
       <c r="FA2" t="s">
-        <v>135</v>
+        <v>561</v>
       </c>
       <c r="FB2" t="s">
-        <v>135</v>
+        <v>560</v>
       </c>
       <c r="FC2" t="s">
-        <v>135</v>
+        <v>523</v>
       </c>
       <c r="FD2" t="s">
-        <v>135</v>
+        <v>562</v>
       </c>
       <c r="FE2" t="s">
-        <v>135</v>
+        <v>563</v>
       </c>
       <c r="FF2" t="s">
-        <v>135</v>
+        <v>530</v>
       </c>
       <c r="FG2" t="s">
-        <v>135</v>
+        <v>557</v>
       </c>
       <c r="FH2" t="s">
-        <v>135</v>
+        <v>564</v>
       </c>
       <c r="FI2" t="s">
-        <v>135</v>
+        <v>565</v>
       </c>
       <c r="FJ2" t="s">
-        <v>135</v>
+        <v>561</v>
       </c>
       <c r="FK2" t="s">
-        <v>135</v>
+        <v>566</v>
       </c>
       <c r="FL2" t="s">
-        <v>135</v>
+        <v>567</v>
       </c>
       <c r="FM2" t="s">
-        <v>135</v>
+        <v>557</v>
       </c>
       <c r="FN2" t="s">
-        <v>135</v>
+        <v>568</v>
       </c>
       <c r="FO2" t="s">
-        <v>135</v>
+        <v>526</v>
       </c>
       <c r="FP2" t="s">
-        <v>135</v>
+        <v>569</v>
       </c>
       <c r="FQ2" t="s">
-        <v>135</v>
+        <v>560</v>
       </c>
       <c r="FR2" t="s">
-        <v>135</v>
+        <v>565</v>
       </c>
       <c r="FS2" t="s">
-        <v>135</v>
+        <v>557</v>
       </c>
       <c r="FT2" t="s">
-        <v>135</v>
+        <v>570</v>
       </c>
       <c r="FU2" t="s">
-        <v>135</v>
+        <v>565</v>
       </c>
       <c r="FV2" t="s">
-        <v>135</v>
+        <v>561</v>
       </c>
       <c r="FW2" t="s">
-        <v>135</v>
+        <v>571</v>
       </c>
       <c r="FX2" t="s">
-        <v>135</v>
+        <v>567</v>
       </c>
       <c r="FY2" t="s">
-        <v>135</v>
+        <v>557</v>
       </c>
       <c r="FZ2" t="s">
-        <v>135</v>
+        <v>572</v>
       </c>
       <c r="GA2" t="s">
-        <v>135</v>
+        <v>565</v>
       </c>
       <c r="GB2" t="s">
-        <v>135</v>
+        <v>562</v>
       </c>
       <c r="GC2" t="s">
         <v>135</v>
@@ -3906,7 +4131,7 @@
         <v>135</v>
       </c>
       <c r="GE2" t="s">
-        <v>135</v>
+        <v>557</v>
       </c>
       <c r="GF2" t="s">
         <v>135</v>
@@ -3915,7 +4140,7 @@
         <v>135</v>
       </c>
       <c r="GH2" t="s">
-        <v>135</v>
+        <v>561</v>
       </c>
       <c r="GI2" t="s">
         <v>135</v>
@@ -3924,7 +4149,7 @@
         <v>135</v>
       </c>
       <c r="GK2" t="s">
-        <v>135</v>
+        <v>569</v>
       </c>
       <c r="GL2" t="s">
         <v>135</v>
@@ -3933,7 +4158,7 @@
         <v>135</v>
       </c>
       <c r="GN2" t="s">
-        <v>135</v>
+        <v>562</v>
       </c>
       <c r="GO2" t="s">
         <v>135</v>
@@ -3942,7 +4167,7 @@
         <v>135</v>
       </c>
       <c r="GQ2" t="s">
-        <v>135</v>
+        <v>562</v>
       </c>
       <c r="GR2" t="s">
         <v>135</v>
@@ -3951,7 +4176,7 @@
         <v>135</v>
       </c>
       <c r="GT2" t="s">
-        <v>135</v>
+        <v>557</v>
       </c>
       <c r="GU2" t="s">
         <v>135</v>
@@ -3960,7 +4185,7 @@
         <v>135</v>
       </c>
       <c r="GW2" t="s">
-        <v>135</v>
+        <v>569</v>
       </c>
       <c r="GX2" t="s">
         <v>135</v>
@@ -3969,55 +4194,55 @@
         <v>135</v>
       </c>
       <c r="GZ2" t="s">
-        <v>135</v>
+        <v>573</v>
       </c>
       <c r="HA2" t="s">
-        <v>135</v>
+        <v>510</v>
       </c>
       <c r="HB2" t="s">
-        <v>135</v>
+        <v>574</v>
       </c>
       <c r="HC2" t="s">
-        <v>135</v>
+        <v>575</v>
       </c>
       <c r="HD2" t="s">
-        <v>135</v>
+        <v>576</v>
       </c>
       <c r="HE2" t="s">
         <v>135</v>
       </c>
       <c r="HF2" t="s">
-        <v>135</v>
+        <v>577</v>
       </c>
       <c r="HG2" t="s">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="HH2" t="s">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="HI2" t="s">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="HJ2" t="s">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="HK2" t="s">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="HL2" t="s">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="HM2" t="s">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="HN2" t="s">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="HO2" t="s">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="HP2" t="s">
-        <v>502</v>
+        <v>135</v>
       </c>
       <c r="HQ2" t="s">
         <v>135</v>
@@ -4149,28 +4374,28 @@
         <v>135</v>
       </c>
       <c r="JH2" t="s">
-        <v>135</v>
+        <v>577</v>
       </c>
       <c r="JI2" t="s">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="JJ2" t="s">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="JK2" t="s">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="JL2" t="s">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="JM2" t="s">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="JN2" t="s">
-        <v>502</v>
+        <v>577</v>
       </c>
       <c r="JO2" t="s">
-        <v>502</v>
+        <v>135</v>
       </c>
       <c r="JP2" t="s">
         <v>135</v>
@@ -4236,52 +4461,52 @@
         <v>135</v>
       </c>
       <c r="KK2" t="s">
-        <v>135</v>
+        <v>578</v>
       </c>
       <c r="KL2" t="s">
-        <v>503</v>
+        <v>135</v>
       </c>
       <c r="KM2" t="s">
-        <v>135</v>
+        <v>577</v>
       </c>
       <c r="KN2" t="s">
-        <v>502</v>
+        <v>135</v>
       </c>
       <c r="KO2" t="s">
-        <v>135</v>
+        <v>579</v>
       </c>
       <c r="KP2" t="s">
-        <v>504</v>
+        <v>135</v>
       </c>
       <c r="KQ2" t="s">
-        <v>135</v>
+        <v>577</v>
       </c>
       <c r="KR2" t="s">
-        <v>502</v>
+        <v>135</v>
       </c>
       <c r="KS2" t="s">
-        <v>135</v>
+        <v>578</v>
       </c>
       <c r="KT2" t="s">
-        <v>503</v>
+        <v>135</v>
       </c>
       <c r="KU2" t="s">
-        <v>135</v>
+        <v>577</v>
       </c>
       <c r="KV2" t="s">
-        <v>502</v>
+        <v>135</v>
       </c>
       <c r="KW2" t="s">
-        <v>135</v>
+        <v>580</v>
       </c>
       <c r="KX2" t="s">
-        <v>505</v>
+        <v>135</v>
       </c>
       <c r="KY2" t="s">
-        <v>135</v>
+        <v>577</v>
       </c>
       <c r="KZ2" t="s">
-        <v>502</v>
+        <v>135</v>
       </c>
       <c r="LA2" t="s">
         <v>135</v>
@@ -4290,10 +4515,7 @@
         <v>135</v>
       </c>
       <c r="LC2" t="s">
-        <v>135</v>
-      </c>
-      <c r="LD2" t="s">
-        <v>506</v>
+        <v>581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Several bugfixes - meeting CST 15.05.2017
</commit_message>
<xml_diff>
--- a/TFG/res/pacientData/1234/Resultats.xlsx
+++ b/TFG/res/pacientData/1234/Resultats.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="654">
   <si>
     <t>Pacient</t>
   </si>
@@ -410,6 +410,9 @@
     <t>CRC total</t>
   </si>
   <si>
+    <t>CRC Rang</t>
+  </si>
+  <si>
     <t>TAP total</t>
   </si>
   <si>
@@ -419,6 +422,9 @@
     <t>MMSE total</t>
   </si>
   <si>
+    <t>MMSE Comentarios</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -1769,9 +1775,42 @@
     <t>adfgadfgag</t>
   </si>
   <si>
+    <t>sdfasdf</t>
+  </si>
+  <si>
+    <t>11/05/2017</t>
+  </si>
+  <si>
+    <t>asdfasdf</t>
+  </si>
+  <si>
+    <t>asdfasf</t>
+  </si>
+  <si>
+    <t>19/05/2017</t>
+  </si>
+  <si>
+    <t>09/05/2017</t>
+  </si>
+  <si>
+    <t>10/05/2017</t>
+  </si>
+  <si>
+    <t>asdfasdfasdfaf</t>
+  </si>
+  <si>
+    <t>24/05/2017</t>
+  </si>
+  <si>
+    <t>pet</t>
+  </si>
+  <si>
     <t>3,0 (Deteriorament greu)</t>
   </si>
   <si>
+    <t>Rang inferior</t>
+  </si>
+  <si>
     <t>20</t>
   </si>
   <si>
@@ -1781,10 +1820,115 @@
     <t>22</t>
   </si>
   <si>
+    <t>72-81</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>90-94</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>44763</t>
+  </si>
+  <si>
+    <t>0.42053</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
-    <t>23</t>
+    <t>46952</t>
+  </si>
+  <si>
+    <t>0.70167</t>
+  </si>
+  <si>
+    <t>37549</t>
+  </si>
+  <si>
+    <t>104720</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>246102</t>
+  </si>
+  <si>
+    <t>0.10739</t>
+  </si>
+  <si>
+    <t>133615</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>268804</t>
+  </si>
+  <si>
+    <t>0.08108</t>
+  </si>
+  <si>
+    <t>112080</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>308798</t>
+  </si>
+  <si>
+    <t>0.13869</t>
+  </si>
+  <si>
+    <t>0.91174</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>296097</t>
+  </si>
+  <si>
+    <t>0.15355</t>
+  </si>
+  <si>
+    <t>105427</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>368781</t>
+  </si>
+  <si>
+    <t>0.14723</t>
+  </si>
+  <si>
+    <t>0.91966</t>
+  </si>
+  <si>
+    <t>76201</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>3-5</t>
+  </si>
+  <si>
+    <t>4.0</t>
   </si>
   <si>
     <t>00:04.83</t>
@@ -1797,6 +1941,39 @@
   </si>
   <si>
     <t>adfg</t>
+  </si>
+  <si>
+    <t>sdfgsdg</t>
+  </si>
+  <si>
+    <t>sdfgsdfg</t>
+  </si>
+  <si>
+    <t>sdfg</t>
+  </si>
+  <si>
+    <t>11-18</t>
+  </si>
+  <si>
+    <t>60-71</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>19-28</t>
+  </si>
+  <si>
+    <t>00:00:00</t>
+  </si>
+  <si>
+    <t>444</t>
   </si>
 </sst>
 </file>
@@ -2803,13 +2980,13 @@
         <v>240</v>
       </c>
       <c r="LG1" t="s">
-        <v>135</v>
+        <v>241</v>
       </c>
       <c r="LH1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="LI1" t="s">
-        <v>242</v>
+        <v>137</v>
       </c>
       <c r="LJ1" t="s">
         <v>243</v>
@@ -2845,40 +3022,40 @@
         <v>253</v>
       </c>
       <c r="LU1" t="s">
-        <v>135</v>
+        <v>254</v>
       </c>
       <c r="LV1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="LW1" t="s">
-        <v>255</v>
+        <v>137</v>
       </c>
       <c r="LX1" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="LY1" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="LZ1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="MA1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="MB1" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="MC1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="MD1" t="s">
-        <v>135</v>
+        <v>252</v>
       </c>
       <c r="ME1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="MF1" t="s">
-        <v>260</v>
+        <v>137</v>
       </c>
       <c r="MG1" t="s">
         <v>261</v>
@@ -3190,13 +3367,13 @@
         <v>363</v>
       </c>
       <c r="QF1" t="s">
-        <v>135</v>
+        <v>364</v>
       </c>
       <c r="QG1" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="QH1" t="s">
-        <v>365</v>
+        <v>137</v>
       </c>
       <c r="QI1" t="s">
         <v>366</v>
@@ -3232,40 +3409,40 @@
         <v>376</v>
       </c>
       <c r="QT1" t="s">
-        <v>135</v>
+        <v>377</v>
       </c>
       <c r="QU1" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="QV1" t="s">
-        <v>378</v>
+        <v>137</v>
       </c>
       <c r="QW1" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="QX1" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="QY1" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="QZ1" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="RA1" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
       <c r="RB1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="RC1" t="s">
-        <v>135</v>
+        <v>375</v>
       </c>
       <c r="RD1" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="RE1" t="s">
-        <v>383</v>
+        <v>137</v>
       </c>
       <c r="RF1" t="s">
         <v>384</v>
@@ -3577,13 +3754,13 @@
         <v>486</v>
       </c>
       <c r="VE1" t="s">
-        <v>135</v>
+        <v>487</v>
       </c>
       <c r="VF1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="VG1" t="s">
-        <v>488</v>
+        <v>137</v>
       </c>
       <c r="VH1" t="s">
         <v>489</v>
@@ -3619,978 +3796,1728 @@
         <v>499</v>
       </c>
       <c r="VS1" t="s">
-        <v>135</v>
+        <v>500</v>
       </c>
       <c r="VT1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="VU1" t="s">
-        <v>501</v>
+        <v>137</v>
       </c>
       <c r="VV1" t="s">
-        <v>493</v>
+        <v>502</v>
       </c>
       <c r="VW1" t="s">
-        <v>494</v>
+        <v>503</v>
       </c>
       <c r="VX1" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="VY1" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="VZ1" t="s">
-        <v>496</v>
+        <v>504</v>
       </c>
       <c r="WA1" t="s">
-        <v>504</v>
+        <v>505</v>
+      </c>
+      <c r="WB1" t="s">
+        <v>498</v>
+      </c>
+      <c r="WC1" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="B2" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C2" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="D2" t="s">
+        <v>509</v>
+      </c>
+      <c r="E2" t="s">
+        <v>510</v>
+      </c>
+      <c r="F2" t="s">
+        <v>511</v>
+      </c>
+      <c r="G2" t="s">
+        <v>512</v>
+      </c>
+      <c r="H2" t="s">
+        <v>513</v>
+      </c>
+      <c r="I2" t="s">
+        <v>514</v>
+      </c>
+      <c r="J2" t="s">
+        <v>515</v>
+      </c>
+      <c r="K2" t="s">
+        <v>516</v>
+      </c>
+      <c r="L2" t="s">
+        <v>517</v>
+      </c>
+      <c r="M2" t="s">
+        <v>518</v>
+      </c>
+      <c r="N2" t="s">
+        <v>519</v>
+      </c>
+      <c r="O2" t="s">
+        <v>520</v>
+      </c>
+      <c r="P2" t="s">
+        <v>521</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>522</v>
+      </c>
+      <c r="R2" t="s">
+        <v>517</v>
+      </c>
+      <c r="S2" t="s">
+        <v>523</v>
+      </c>
+      <c r="T2" t="s">
+        <v>524</v>
+      </c>
+      <c r="U2" t="s">
+        <v>525</v>
+      </c>
+      <c r="V2" t="s">
+        <v>526</v>
+      </c>
+      <c r="W2" t="s">
+        <v>527</v>
+      </c>
+      <c r="X2" t="s">
+        <v>522</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>522</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>522</v>
+      </c>
+      <c r="AA2" t="s">
         <v>507</v>
       </c>
-      <c r="E2" t="s">
-        <v>508</v>
-      </c>
-      <c r="F2" t="s">
-        <v>509</v>
-      </c>
-      <c r="G2" t="s">
-        <v>510</v>
-      </c>
-      <c r="H2" t="s">
-        <v>511</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="AB2" t="s">
+        <v>528</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>529</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>530</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>519</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>519</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>519</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>522</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>531</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>532</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>522</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>522</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>534</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>522</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>518</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>522</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>535</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>522</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>536</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>522</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>535</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>522</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>535</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>522</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>537</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>522</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>538</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>522</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>538</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>522</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>535</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>522</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>533</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>522</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>539</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>522</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>535</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>522</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>535</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>522</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>540</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>522</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>539</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>522</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>541</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>518</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>522</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>518</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>518</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>522</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>522</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>518</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>522</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>542</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>522</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>538</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>518</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>522</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>543</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>518</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>522</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>539</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>518</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>522</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>544</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>522</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>539</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>522</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>540</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>522</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>544</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>518</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>518</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>518</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>545</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>546</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>547</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>548</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>549</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>550</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>551</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>552</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>553</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>554</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>555</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>556</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>557</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>558</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>559</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>560</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>561</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>562</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>563</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>564</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>565</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>566</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>567</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>519</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>520</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>521</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>517</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>524</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>525</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>526</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>568</v>
+      </c>
+      <c r="ER2" t="s">
+        <v>569</v>
+      </c>
+      <c r="ES2" t="s">
         <v>512</v>
       </c>
-      <c r="J2" t="s">
-        <v>513</v>
-      </c>
-      <c r="K2" t="s">
-        <v>514</v>
-      </c>
-      <c r="L2" t="s">
-        <v>515</v>
-      </c>
-      <c r="M2" t="s">
-        <v>516</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="ET2" t="s">
+        <v>570</v>
+      </c>
+      <c r="EU2" t="s">
+        <v>571</v>
+      </c>
+      <c r="EV2" t="s">
+        <v>572</v>
+      </c>
+      <c r="EW2" t="s">
+        <v>573</v>
+      </c>
+      <c r="EX2" t="s">
+        <v>571</v>
+      </c>
+      <c r="EY2" t="s">
+        <v>574</v>
+      </c>
+      <c r="EZ2" t="s">
+        <v>539</v>
+      </c>
+      <c r="FA2" t="s">
+        <v>575</v>
+      </c>
+      <c r="FB2" t="s">
+        <v>574</v>
+      </c>
+      <c r="FC2" t="s">
+        <v>537</v>
+      </c>
+      <c r="FD2" t="s">
+        <v>576</v>
+      </c>
+      <c r="FE2" t="s">
+        <v>577</v>
+      </c>
+      <c r="FF2" t="s">
+        <v>544</v>
+      </c>
+      <c r="FG2" t="s">
+        <v>571</v>
+      </c>
+      <c r="FH2" t="s">
+        <v>578</v>
+      </c>
+      <c r="FI2" t="s">
+        <v>579</v>
+      </c>
+      <c r="FJ2" t="s">
+        <v>575</v>
+      </c>
+      <c r="FK2" t="s">
+        <v>580</v>
+      </c>
+      <c r="FL2" t="s">
+        <v>581</v>
+      </c>
+      <c r="FM2" t="s">
+        <v>571</v>
+      </c>
+      <c r="FN2" t="s">
+        <v>582</v>
+      </c>
+      <c r="FO2" t="s">
+        <v>540</v>
+      </c>
+      <c r="FP2" t="s">
+        <v>583</v>
+      </c>
+      <c r="FQ2" t="s">
+        <v>574</v>
+      </c>
+      <c r="FR2" t="s">
+        <v>579</v>
+      </c>
+      <c r="FS2" t="s">
+        <v>571</v>
+      </c>
+      <c r="FT2" t="s">
+        <v>584</v>
+      </c>
+      <c r="FU2" t="s">
+        <v>579</v>
+      </c>
+      <c r="FV2" t="s">
+        <v>575</v>
+      </c>
+      <c r="FW2" t="s">
+        <v>585</v>
+      </c>
+      <c r="FX2" t="s">
+        <v>581</v>
+      </c>
+      <c r="FY2" t="s">
+        <v>571</v>
+      </c>
+      <c r="FZ2" t="s">
+        <v>586</v>
+      </c>
+      <c r="GA2" t="s">
+        <v>579</v>
+      </c>
+      <c r="GB2" t="s">
+        <v>576</v>
+      </c>
+      <c r="GC2" t="s">
+        <v>587</v>
+      </c>
+      <c r="GD2" t="s">
+        <v>588</v>
+      </c>
+      <c r="GE2" t="s">
+        <v>576</v>
+      </c>
+      <c r="GF2" t="s">
+        <v>589</v>
+      </c>
+      <c r="GG2" t="s">
+        <v>588</v>
+      </c>
+      <c r="GH2" t="s">
+        <v>571</v>
+      </c>
+      <c r="GI2" t="s">
+        <v>590</v>
+      </c>
+      <c r="GJ2" t="s">
+        <v>591</v>
+      </c>
+      <c r="GK2" t="s">
+        <v>571</v>
+      </c>
+      <c r="GL2" t="s">
+        <v>589</v>
+      </c>
+      <c r="GM2" t="s">
+        <v>592</v>
+      </c>
+      <c r="GN2" t="s">
+        <v>575</v>
+      </c>
+      <c r="GO2" t="s">
+        <v>589</v>
+      </c>
+      <c r="GP2" t="s">
+        <v>593</v>
+      </c>
+      <c r="GQ2" t="s">
+        <v>571</v>
+      </c>
+      <c r="GR2" t="s">
+        <v>589</v>
+      </c>
+      <c r="GS2" t="s">
+        <v>592</v>
+      </c>
+      <c r="GT2" t="s">
+        <v>575</v>
+      </c>
+      <c r="GU2" t="s">
+        <v>594</v>
+      </c>
+      <c r="GV2" t="s">
+        <v>595</v>
+      </c>
+      <c r="GW2" t="s">
+        <v>571</v>
+      </c>
+      <c r="GX2" t="s">
+        <v>596</v>
+      </c>
+      <c r="GY2" t="s">
+        <v>592</v>
+      </c>
+      <c r="GZ2" t="s">
+        <v>597</v>
+      </c>
+      <c r="HA2" t="s">
+        <v>524</v>
+      </c>
+      <c r="HB2" t="s">
+        <v>598</v>
+      </c>
+      <c r="HC2" t="s">
+        <v>599</v>
+      </c>
+      <c r="HD2" t="s">
+        <v>600</v>
+      </c>
+      <c r="HE2" t="s">
+        <v>601</v>
+      </c>
+      <c r="HF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HH2" t="s">
+        <v>525</v>
+      </c>
+      <c r="HI2" t="s">
+        <v>512</v>
+      </c>
+      <c r="HJ2" t="s">
+        <v>602</v>
+      </c>
+      <c r="HK2" t="s">
+        <v>603</v>
+      </c>
+      <c r="HL2" t="s">
+        <v>524</v>
+      </c>
+      <c r="HM2" t="s">
+        <v>512</v>
+      </c>
+      <c r="HN2" t="s">
+        <v>604</v>
+      </c>
+      <c r="HO2" t="s">
+        <v>605</v>
+      </c>
+      <c r="HP2" t="s">
+        <v>606</v>
+      </c>
+      <c r="HQ2" t="s">
+        <v>570</v>
+      </c>
+      <c r="HR2" t="s">
+        <v>607</v>
+      </c>
+      <c r="HS2" t="s">
+        <v>608</v>
+      </c>
+      <c r="HT2" t="s">
+        <v>520</v>
+      </c>
+      <c r="HU2" t="s">
+        <v>609</v>
+      </c>
+      <c r="HV2" t="s">
+        <v>603</v>
+      </c>
+      <c r="HW2" t="s">
+        <v>610</v>
+      </c>
+      <c r="HX2" t="s">
+        <v>611</v>
+      </c>
+      <c r="HY2" t="s">
+        <v>524</v>
+      </c>
+      <c r="HZ2" t="s">
+        <v>609</v>
+      </c>
+      <c r="IA2" t="s">
+        <v>603</v>
+      </c>
+      <c r="IB2" t="s">
+        <v>612</v>
+      </c>
+      <c r="IC2" t="s">
+        <v>613</v>
+      </c>
+      <c r="ID2" t="s">
+        <v>569</v>
+      </c>
+      <c r="IE2" t="s">
+        <v>609</v>
+      </c>
+      <c r="IF2" t="s">
+        <v>603</v>
+      </c>
+      <c r="IG2" t="s">
+        <v>614</v>
+      </c>
+      <c r="IH2" t="s">
+        <v>520</v>
+      </c>
+      <c r="II2" t="s">
+        <v>615</v>
+      </c>
+      <c r="IJ2" t="s">
+        <v>616</v>
+      </c>
+      <c r="IK2" t="s">
+        <v>617</v>
+      </c>
+      <c r="IL2" t="s">
+        <v>618</v>
+      </c>
+      <c r="IM2" t="s">
+        <v>526</v>
+      </c>
+      <c r="IN2" t="s">
+        <v>619</v>
+      </c>
+      <c r="IO2" t="s">
+        <v>620</v>
+      </c>
+      <c r="IP2" t="s">
+        <v>621</v>
+      </c>
+      <c r="IQ2" t="s">
+        <v>622</v>
+      </c>
+      <c r="IR2" t="s">
+        <v>623</v>
+      </c>
+      <c r="IS2" t="s">
+        <v>624</v>
+      </c>
+      <c r="IT2" t="s">
+        <v>625</v>
+      </c>
+      <c r="IU2" t="s">
+        <v>626</v>
+      </c>
+      <c r="IV2" t="s">
+        <v>627</v>
+      </c>
+      <c r="IW2" t="s">
+        <v>512</v>
+      </c>
+      <c r="IX2" t="s">
+        <v>628</v>
+      </c>
+      <c r="IY2" t="s">
+        <v>629</v>
+      </c>
+      <c r="IZ2" t="s">
+        <v>630</v>
+      </c>
+      <c r="JA2" t="s">
+        <v>627</v>
+      </c>
+      <c r="JB2" t="s">
+        <v>631</v>
+      </c>
+      <c r="JC2" t="s">
+        <v>632</v>
+      </c>
+      <c r="JD2" t="s">
+        <v>633</v>
+      </c>
+      <c r="JE2" t="s">
+        <v>634</v>
+      </c>
+      <c r="JF2" t="s">
+        <v>524</v>
+      </c>
+      <c r="JG2" t="s">
+        <v>520</v>
+      </c>
+      <c r="JH2" t="s">
+        <v>611</v>
+      </c>
+      <c r="JI2" t="s">
+        <v>635</v>
+      </c>
+      <c r="JJ2" t="s">
+        <v>636</v>
+      </c>
+      <c r="JK2" t="s">
+        <v>609</v>
+      </c>
+      <c r="JL2" t="s">
+        <v>609</v>
+      </c>
+      <c r="JM2" t="s">
+        <v>568</v>
+      </c>
+      <c r="JN2" t="s">
+        <v>609</v>
+      </c>
+      <c r="JO2" t="s">
+        <v>637</v>
+      </c>
+      <c r="JP2" t="s">
+        <v>524</v>
+      </c>
+      <c r="JQ2" t="s">
+        <v>519</v>
+      </c>
+      <c r="JR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KA2" t="s">
+        <v>524</v>
+      </c>
+      <c r="KB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KK2" t="s">
+        <v>638</v>
+      </c>
+      <c r="KL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KM2" t="s">
+        <v>639</v>
+      </c>
+      <c r="KN2" t="s">
+        <v>521</v>
+      </c>
+      <c r="KO2" t="s">
+        <v>609</v>
+      </c>
+      <c r="KP2" t="s">
+        <v>521</v>
+      </c>
+      <c r="KQ2" t="s">
+        <v>640</v>
+      </c>
+      <c r="KR2" t="s">
+        <v>521</v>
+      </c>
+      <c r="KS2" t="s">
+        <v>609</v>
+      </c>
+      <c r="KT2" t="s">
+        <v>521</v>
+      </c>
+      <c r="KU2" t="s">
+        <v>639</v>
+      </c>
+      <c r="KV2" t="s">
+        <v>521</v>
+      </c>
+      <c r="KW2" t="s">
+        <v>609</v>
+      </c>
+      <c r="KX2" t="s">
+        <v>521</v>
+      </c>
+      <c r="KY2" t="s">
+        <v>641</v>
+      </c>
+      <c r="KZ2" t="s">
+        <v>521</v>
+      </c>
+      <c r="LA2" t="s">
+        <v>609</v>
+      </c>
+      <c r="LB2" t="s">
+        <v>521</v>
+      </c>
+      <c r="LC2" t="s">
+        <v>521</v>
+      </c>
+      <c r="LD2" t="s">
+        <v>521</v>
+      </c>
+      <c r="LE2" t="s">
+        <v>642</v>
+      </c>
+      <c r="LF2" t="s">
+        <v>643</v>
+      </c>
+      <c r="LG2" t="s">
+        <v>644</v>
+      </c>
+      <c r="LH2" t="s">
+        <v>645</v>
+      </c>
+      <c r="LI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MD2" t="s">
         <v>517</v>
       </c>
-      <c r="O2" t="s">
-        <v>518</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="ME2" t="s">
+        <v>525</v>
+      </c>
+      <c r="MF2" t="s">
+        <v>646</v>
+      </c>
+      <c r="MG2" t="s">
+        <v>526</v>
+      </c>
+      <c r="MH2" t="s">
+        <v>517</v>
+      </c>
+      <c r="MI2" t="s">
+        <v>568</v>
+      </c>
+      <c r="MJ2" t="s">
+        <v>647</v>
+      </c>
+      <c r="MK2" t="s">
+        <v>570</v>
+      </c>
+      <c r="ML2" t="s">
+        <v>648</v>
+      </c>
+      <c r="MM2" t="s">
+        <v>569</v>
+      </c>
+      <c r="MN2" t="s">
+        <v>607</v>
+      </c>
+      <c r="MO2" t="s">
+        <v>608</v>
+      </c>
+      <c r="MP2" t="s">
+        <v>520</v>
+      </c>
+      <c r="MQ2" t="s">
+        <v>609</v>
+      </c>
+      <c r="MR2" t="s">
+        <v>603</v>
+      </c>
+      <c r="MS2" t="s">
+        <v>610</v>
+      </c>
+      <c r="MT2" t="s">
+        <v>611</v>
+      </c>
+      <c r="MU2" t="s">
+        <v>524</v>
+      </c>
+      <c r="MV2" t="s">
+        <v>609</v>
+      </c>
+      <c r="MW2" t="s">
+        <v>603</v>
+      </c>
+      <c r="MX2" t="s">
+        <v>612</v>
+      </c>
+      <c r="MY2" t="s">
+        <v>613</v>
+      </c>
+      <c r="MZ2" t="s">
+        <v>569</v>
+      </c>
+      <c r="NA2" t="s">
+        <v>609</v>
+      </c>
+      <c r="NB2" t="s">
+        <v>603</v>
+      </c>
+      <c r="NC2" t="s">
+        <v>614</v>
+      </c>
+      <c r="ND2" t="s">
+        <v>520</v>
+      </c>
+      <c r="NE2" t="s">
+        <v>615</v>
+      </c>
+      <c r="NF2" t="s">
+        <v>616</v>
+      </c>
+      <c r="NG2" t="s">
+        <v>617</v>
+      </c>
+      <c r="NH2" t="s">
+        <v>618</v>
+      </c>
+      <c r="NI2" t="s">
+        <v>526</v>
+      </c>
+      <c r="NJ2" t="s">
+        <v>619</v>
+      </c>
+      <c r="NK2" t="s">
+        <v>620</v>
+      </c>
+      <c r="NL2" t="s">
+        <v>621</v>
+      </c>
+      <c r="NM2" t="s">
+        <v>622</v>
+      </c>
+      <c r="NN2" t="s">
+        <v>623</v>
+      </c>
+      <c r="NO2" t="s">
+        <v>624</v>
+      </c>
+      <c r="NP2" t="s">
+        <v>625</v>
+      </c>
+      <c r="NQ2" t="s">
+        <v>626</v>
+      </c>
+      <c r="NR2" t="s">
+        <v>627</v>
+      </c>
+      <c r="NS2" t="s">
+        <v>512</v>
+      </c>
+      <c r="NT2" t="s">
+        <v>628</v>
+      </c>
+      <c r="NU2" t="s">
+        <v>629</v>
+      </c>
+      <c r="NV2" t="s">
+        <v>630</v>
+      </c>
+      <c r="NW2" t="s">
+        <v>627</v>
+      </c>
+      <c r="NX2" t="s">
+        <v>631</v>
+      </c>
+      <c r="NY2" t="s">
+        <v>632</v>
+      </c>
+      <c r="NZ2" t="s">
+        <v>633</v>
+      </c>
+      <c r="OA2" t="s">
+        <v>634</v>
+      </c>
+      <c r="OB2" t="s">
+        <v>524</v>
+      </c>
+      <c r="OC2" t="s">
+        <v>520</v>
+      </c>
+      <c r="OD2" t="s">
+        <v>611</v>
+      </c>
+      <c r="OE2" t="s">
+        <v>635</v>
+      </c>
+      <c r="OF2" t="s">
+        <v>649</v>
+      </c>
+      <c r="OG2" t="s">
+        <v>512</v>
+      </c>
+      <c r="OH2" t="s">
+        <v>650</v>
+      </c>
+      <c r="OI2" t="s">
+        <v>570</v>
+      </c>
+      <c r="OJ2" t="s">
+        <v>517</v>
+      </c>
+      <c r="OK2" t="s">
+        <v>651</v>
+      </c>
+      <c r="OL2" t="s">
+        <v>568</v>
+      </c>
+      <c r="OM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ON2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PI2" t="s">
+        <v>652</v>
+      </c>
+      <c r="PJ2" t="s">
         <v>519</v>
       </c>
-      <c r="Q2" t="s">
-        <v>520</v>
-      </c>
-      <c r="R2" t="s">
-        <v>515</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="PK2" t="s">
+        <v>609</v>
+      </c>
+      <c r="PL2" t="s">
+        <v>519</v>
+      </c>
+      <c r="PM2" t="s">
+        <v>652</v>
+      </c>
+      <c r="PN2" t="s">
+        <v>519</v>
+      </c>
+      <c r="PO2" t="s">
+        <v>609</v>
+      </c>
+      <c r="PP2" t="s">
+        <v>519</v>
+      </c>
+      <c r="PQ2" t="s">
+        <v>652</v>
+      </c>
+      <c r="PR2" t="s">
+        <v>519</v>
+      </c>
+      <c r="PS2" t="s">
+        <v>609</v>
+      </c>
+      <c r="PT2" t="s">
+        <v>519</v>
+      </c>
+      <c r="PU2" t="s">
+        <v>652</v>
+      </c>
+      <c r="PV2" t="s">
+        <v>519</v>
+      </c>
+      <c r="PW2" t="s">
+        <v>609</v>
+      </c>
+      <c r="PX2" t="s">
+        <v>519</v>
+      </c>
+      <c r="PY2" t="s">
+        <v>519</v>
+      </c>
+      <c r="PZ2" t="s">
+        <v>519</v>
+      </c>
+      <c r="QA2" t="s">
+        <v>653</v>
+      </c>
+      <c r="QB2" t="s">
+        <v>653</v>
+      </c>
+      <c r="QC2" t="s">
+        <v>653</v>
+      </c>
+      <c r="QD2" t="s">
+        <v>653</v>
+      </c>
+      <c r="QE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QX2" t="s">
+        <v>517</v>
+      </c>
+      <c r="QY2" t="s">
+        <v>525</v>
+      </c>
+      <c r="QZ2" t="s">
+        <v>646</v>
+      </c>
+      <c r="RA2" t="s">
+        <v>526</v>
+      </c>
+      <c r="RB2" t="s">
+        <v>609</v>
+      </c>
+      <c r="RC2" t="s">
+        <v>609</v>
+      </c>
+      <c r="RD2" t="s">
+        <v>609</v>
+      </c>
+      <c r="RE2" t="s">
+        <v>609</v>
+      </c>
+      <c r="RF2" t="s">
         <v>521</v>
       </c>
-      <c r="T2" t="s">
-        <v>522</v>
-      </c>
-      <c r="U2" t="s">
-        <v>523</v>
-      </c>
-      <c r="V2" t="s">
-        <v>524</v>
-      </c>
-      <c r="W2" t="s">
-        <v>525</v>
-      </c>
-      <c r="X2" t="s">
-        <v>520</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>520</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>520</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>505</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>526</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>527</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>528</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>517</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>517</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>517</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>520</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>529</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>530</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>520</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>531</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>520</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>532</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>520</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>531</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>516</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>520</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>533</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>520</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>534</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>520</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>533</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>520</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>533</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>520</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>535</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>520</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>536</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>520</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>536</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>520</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>533</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>520</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>531</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>520</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>537</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>520</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>533</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>520</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>533</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>520</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>538</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>520</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>537</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>520</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>539</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>516</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>135</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>520</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>135</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>516</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>135</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>516</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>135</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>520</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>135</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>520</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>135</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>516</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>135</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>520</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>540</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>520</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>536</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>516</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>135</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>520</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>541</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>516</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>135</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>520</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>537</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>516</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>135</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>520</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>542</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>520</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>537</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>520</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>538</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>520</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>542</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>516</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>135</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>516</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>135</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>516</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>135</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>543</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>544</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>545</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>546</v>
-      </c>
-      <c r="DQ2" t="s">
-        <v>547</v>
-      </c>
-      <c r="DR2" t="s">
-        <v>548</v>
-      </c>
-      <c r="DS2" t="s">
-        <v>549</v>
-      </c>
-      <c r="DT2" t="s">
-        <v>550</v>
-      </c>
-      <c r="DU2" t="s">
-        <v>551</v>
-      </c>
-      <c r="DV2" t="s">
-        <v>552</v>
-      </c>
-      <c r="DW2" t="s">
-        <v>553</v>
-      </c>
-      <c r="DX2" t="s">
-        <v>554</v>
-      </c>
-      <c r="DY2" t="s">
-        <v>555</v>
-      </c>
-      <c r="DZ2" t="s">
-        <v>556</v>
-      </c>
-      <c r="EA2" t="s">
-        <v>557</v>
-      </c>
-      <c r="EB2" t="s">
-        <v>558</v>
-      </c>
-      <c r="EC2" t="s">
-        <v>559</v>
-      </c>
-      <c r="ED2" t="s">
-        <v>560</v>
-      </c>
-      <c r="EE2" t="s">
-        <v>561</v>
-      </c>
-      <c r="EF2" t="s">
-        <v>562</v>
-      </c>
-      <c r="EG2" t="s">
-        <v>563</v>
-      </c>
-      <c r="EH2" t="s">
-        <v>564</v>
-      </c>
-      <c r="EI2" t="s">
-        <v>565</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>517</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>518</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>519</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>515</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>522</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>523</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>524</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>566</v>
-      </c>
-      <c r="ER2" t="s">
-        <v>567</v>
-      </c>
-      <c r="ES2" t="s">
-        <v>510</v>
-      </c>
-      <c r="ET2" t="s">
-        <v>568</v>
-      </c>
-      <c r="EU2" t="s">
-        <v>569</v>
-      </c>
-      <c r="EV2" t="s">
-        <v>570</v>
-      </c>
-      <c r="EW2" t="s">
-        <v>571</v>
-      </c>
-      <c r="EX2" t="s">
-        <v>569</v>
-      </c>
-      <c r="EY2" t="s">
-        <v>572</v>
-      </c>
-      <c r="EZ2" t="s">
-        <v>537</v>
-      </c>
-      <c r="FA2" t="s">
-        <v>573</v>
-      </c>
-      <c r="FB2" t="s">
-        <v>572</v>
-      </c>
-      <c r="FC2" t="s">
-        <v>535</v>
-      </c>
-      <c r="FD2" t="s">
-        <v>574</v>
-      </c>
-      <c r="FE2" t="s">
-        <v>575</v>
-      </c>
-      <c r="FF2" t="s">
-        <v>542</v>
-      </c>
-      <c r="FG2" t="s">
-        <v>569</v>
-      </c>
-      <c r="FH2" t="s">
-        <v>576</v>
-      </c>
-      <c r="FI2" t="s">
-        <v>577</v>
-      </c>
-      <c r="FJ2" t="s">
-        <v>573</v>
-      </c>
-      <c r="FK2" t="s">
-        <v>578</v>
-      </c>
-      <c r="FL2" t="s">
-        <v>579</v>
-      </c>
-      <c r="FM2" t="s">
-        <v>569</v>
-      </c>
-      <c r="FN2" t="s">
-        <v>580</v>
-      </c>
-      <c r="FO2" t="s">
-        <v>538</v>
-      </c>
-      <c r="FP2" t="s">
-        <v>581</v>
-      </c>
-      <c r="FQ2" t="s">
-        <v>572</v>
-      </c>
-      <c r="FR2" t="s">
-        <v>577</v>
-      </c>
-      <c r="FS2" t="s">
-        <v>569</v>
-      </c>
-      <c r="FT2" t="s">
-        <v>582</v>
-      </c>
-      <c r="FU2" t="s">
-        <v>577</v>
-      </c>
-      <c r="FV2" t="s">
-        <v>573</v>
-      </c>
-      <c r="FW2" t="s">
-        <v>583</v>
-      </c>
-      <c r="FX2" t="s">
-        <v>579</v>
-      </c>
-      <c r="FY2" t="s">
-        <v>569</v>
-      </c>
-      <c r="FZ2" t="s">
-        <v>584</v>
-      </c>
-      <c r="GA2" t="s">
-        <v>577</v>
-      </c>
-      <c r="GB2" t="s">
-        <v>574</v>
-      </c>
-      <c r="GC2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GD2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GE2" t="s">
-        <v>569</v>
-      </c>
-      <c r="GF2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GG2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GH2" t="s">
-        <v>573</v>
-      </c>
-      <c r="GI2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GJ2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GK2" t="s">
-        <v>581</v>
-      </c>
-      <c r="GL2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GM2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GN2" t="s">
-        <v>574</v>
-      </c>
-      <c r="GO2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GP2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GQ2" t="s">
-        <v>574</v>
-      </c>
-      <c r="GR2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GS2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GT2" t="s">
-        <v>569</v>
-      </c>
-      <c r="GU2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GV2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GW2" t="s">
-        <v>581</v>
-      </c>
-      <c r="GX2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GY2" t="s">
-        <v>135</v>
-      </c>
-      <c r="GZ2" t="s">
-        <v>585</v>
-      </c>
-      <c r="HA2" t="s">
-        <v>522</v>
-      </c>
-      <c r="HB2" t="s">
-        <v>586</v>
-      </c>
-      <c r="HC2" t="s">
-        <v>587</v>
-      </c>
-      <c r="HD2" t="s">
-        <v>588</v>
-      </c>
-      <c r="HE2" t="s">
-        <v>135</v>
-      </c>
-      <c r="HF2" t="s">
-        <v>589</v>
-      </c>
-      <c r="HG2" t="s">
-        <v>589</v>
-      </c>
-      <c r="HH2" t="s">
-        <v>589</v>
-      </c>
-      <c r="HI2" t="s">
-        <v>589</v>
-      </c>
-      <c r="HJ2" t="s">
-        <v>589</v>
-      </c>
-      <c r="HK2" t="s">
-        <v>589</v>
-      </c>
-      <c r="HL2" t="s">
-        <v>589</v>
-      </c>
-      <c r="HM2" t="s">
-        <v>589</v>
-      </c>
-      <c r="HN2" t="s">
-        <v>590</v>
-      </c>
-      <c r="HO2" t="s">
-        <v>568</v>
-      </c>
-      <c r="HP2" t="s">
-        <v>135</v>
-      </c>
-      <c r="HQ2" t="s">
-        <v>135</v>
-      </c>
-      <c r="HR2" t="s">
-        <v>135</v>
-      </c>
-      <c r="HS2" t="s">
-        <v>135</v>
-      </c>
-      <c r="HT2" t="s">
-        <v>135</v>
-      </c>
-      <c r="HU2" t="s">
-        <v>135</v>
-      </c>
-      <c r="HV2" t="s">
-        <v>135</v>
-      </c>
-      <c r="HW2" t="s">
-        <v>135</v>
-      </c>
-      <c r="HX2" t="s">
-        <v>135</v>
-      </c>
-      <c r="HY2" t="s">
-        <v>135</v>
-      </c>
-      <c r="HZ2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IA2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IB2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IC2" t="s">
-        <v>135</v>
-      </c>
-      <c r="ID2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IE2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IF2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IG2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IH2" t="s">
-        <v>135</v>
-      </c>
-      <c r="II2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IJ2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IK2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IL2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IM2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IN2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IO2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IP2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IQ2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IR2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IS2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IT2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IU2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IV2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IW2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IX2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IY2" t="s">
-        <v>135</v>
-      </c>
-      <c r="IZ2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JA2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JB2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JC2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JD2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JE2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JF2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JG2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JH2" t="s">
-        <v>589</v>
-      </c>
-      <c r="JI2" t="s">
-        <v>589</v>
-      </c>
-      <c r="JJ2" t="s">
-        <v>589</v>
-      </c>
-      <c r="JK2" t="s">
-        <v>589</v>
-      </c>
-      <c r="JL2" t="s">
-        <v>589</v>
-      </c>
-      <c r="JM2" t="s">
-        <v>589</v>
-      </c>
-      <c r="JN2" t="s">
-        <v>589</v>
-      </c>
-      <c r="JO2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JP2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JQ2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JR2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JS2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JT2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JU2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JV2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JW2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JX2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JY2" t="s">
-        <v>135</v>
-      </c>
-      <c r="JZ2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KA2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KB2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KC2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KD2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KE2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KF2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KG2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KH2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KI2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KJ2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KK2" t="s">
-        <v>591</v>
-      </c>
-      <c r="KL2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KM2" t="s">
-        <v>589</v>
-      </c>
-      <c r="KN2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KO2" t="s">
-        <v>592</v>
-      </c>
-      <c r="KP2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KQ2" t="s">
-        <v>589</v>
-      </c>
-      <c r="KR2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KS2" t="s">
-        <v>591</v>
-      </c>
-      <c r="KT2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KU2" t="s">
-        <v>589</v>
-      </c>
-      <c r="KV2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KW2" t="s">
-        <v>593</v>
-      </c>
-      <c r="KX2" t="s">
-        <v>135</v>
-      </c>
-      <c r="KY2" t="s">
-        <v>589</v>
-      </c>
-      <c r="KZ2" t="s">
-        <v>135</v>
-      </c>
-      <c r="LA2" t="s">
-        <v>135</v>
-      </c>
-      <c r="LB2" t="s">
-        <v>135</v>
-      </c>
-      <c r="LC2" t="s">
-        <v>594</v>
+      <c r="RG2" t="s">
+        <v>609</v>
+      </c>
+      <c r="RH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ST2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SZ2" t="s">
+        <v>609</v>
+      </c>
+      <c r="TA2" t="s">
+        <v>609</v>
+      </c>
+      <c r="TB2" t="s">
+        <v>609</v>
+      </c>
+      <c r="TC2" t="s">
+        <v>609</v>
+      </c>
+      <c r="TD2" t="s">
+        <v>609</v>
+      </c>
+      <c r="TE2" t="s">
+        <v>609</v>
+      </c>
+      <c r="TF2" t="s">
+        <v>609</v>
+      </c>
+      <c r="TG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UC2" t="s">
+        <v>652</v>
+      </c>
+      <c r="UD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UE2" t="s">
+        <v>609</v>
+      </c>
+      <c r="UF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UG2" t="s">
+        <v>652</v>
+      </c>
+      <c r="UH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UI2" t="s">
+        <v>609</v>
+      </c>
+      <c r="UJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UK2" t="s">
+        <v>652</v>
+      </c>
+      <c r="UL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UM2" t="s">
+        <v>609</v>
+      </c>
+      <c r="UN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UO2" t="s">
+        <v>652</v>
+      </c>
+      <c r="UP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UQ2" t="s">
+        <v>609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Afegit sistema per controlar noms i ids REM-XXXXX - meeting CST 07.06.2017
</commit_message>
<xml_diff>
--- a/TFG/res/pacientData/1234/Resultats.xlsx
+++ b/TFG/res/pacientData/1234/Resultats.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="655">
   <si>
     <t>Pacient</t>
   </si>
   <si>
-    <t>Codi subjecte</t>
+    <t>Codi aplicació</t>
   </si>
   <si>
     <t>Sexe</t>
@@ -1536,6 +1536,9 @@
   </si>
   <si>
     <t>1234</t>
+  </si>
+  <si>
+    <t>REM-G1234</t>
   </si>
   <si>
     <t>Home</t>
@@ -3834,1690 +3837,1690 @@
         <v>507</v>
       </c>
       <c r="B2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="E2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="F2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="G2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="H2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="I2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="J2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="K2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="L2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="M2" t="s">
+        <v>519</v>
+      </c>
+      <c r="N2" t="s">
+        <v>520</v>
+      </c>
+      <c r="O2" t="s">
+        <v>521</v>
+      </c>
+      <c r="P2" t="s">
+        <v>522</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>523</v>
+      </c>
+      <c r="R2" t="s">
         <v>518</v>
       </c>
-      <c r="N2" t="s">
-        <v>519</v>
-      </c>
-      <c r="O2" t="s">
-        <v>520</v>
-      </c>
-      <c r="P2" t="s">
-        <v>521</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>522</v>
-      </c>
-      <c r="R2" t="s">
-        <v>517</v>
-      </c>
       <c r="S2" t="s">
+        <v>524</v>
+      </c>
+      <c r="T2" t="s">
+        <v>525</v>
+      </c>
+      <c r="U2" t="s">
+        <v>526</v>
+      </c>
+      <c r="V2" t="s">
+        <v>527</v>
+      </c>
+      <c r="W2" t="s">
+        <v>528</v>
+      </c>
+      <c r="X2" t="s">
         <v>523</v>
       </c>
-      <c r="T2" t="s">
-        <v>524</v>
-      </c>
-      <c r="U2" t="s">
-        <v>525</v>
-      </c>
-      <c r="V2" t="s">
-        <v>526</v>
-      </c>
-      <c r="W2" t="s">
-        <v>527</v>
-      </c>
-      <c r="X2" t="s">
-        <v>522</v>
-      </c>
       <c r="Y2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="Z2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="AA2" t="s">
         <v>507</v>
       </c>
       <c r="AB2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="AC2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="AD2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="AE2" t="s">
+        <v>520</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>520</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>520</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>523</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>532</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>533</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>523</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>534</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>523</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>535</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>523</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>534</v>
+      </c>
+      <c r="AQ2" t="s">
         <v>519</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>523</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>536</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>523</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>537</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>523</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>536</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>523</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>536</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>523</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>538</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>523</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>539</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>523</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>539</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>523</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>536</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>523</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>534</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>523</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>540</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>523</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>536</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>523</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>536</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>523</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>541</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>523</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>540</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>523</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>542</v>
+      </c>
+      <c r="BW2" t="s">
         <v>519</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="BX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>523</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CA2" t="s">
         <v>519</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="CB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>519</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>523</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>523</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>519</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>523</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>543</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>523</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>539</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>519</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>523</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>544</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>519</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>523</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>540</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>519</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>523</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>545</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>523</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>540</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>523</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>541</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>523</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>545</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>519</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>519</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>519</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>546</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>547</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>548</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>549</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>550</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>551</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>552</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>553</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>554</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>555</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>556</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>557</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>558</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>559</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>560</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>561</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>562</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>563</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>564</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>565</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>566</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>567</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>568</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>520</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>521</v>
+      </c>
+      <c r="EL2" t="s">
         <v>522</v>
       </c>
-      <c r="AI2" t="s">
-        <v>531</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>532</v>
-      </c>
-      <c r="AK2" t="s">
+      <c r="EM2" t="s">
+        <v>518</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>525</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>526</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>527</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>569</v>
+      </c>
+      <c r="ER2" t="s">
+        <v>570</v>
+      </c>
+      <c r="ES2" t="s">
+        <v>513</v>
+      </c>
+      <c r="ET2" t="s">
+        <v>571</v>
+      </c>
+      <c r="EU2" t="s">
+        <v>572</v>
+      </c>
+      <c r="EV2" t="s">
+        <v>573</v>
+      </c>
+      <c r="EW2" t="s">
+        <v>574</v>
+      </c>
+      <c r="EX2" t="s">
+        <v>572</v>
+      </c>
+      <c r="EY2" t="s">
+        <v>575</v>
+      </c>
+      <c r="EZ2" t="s">
+        <v>540</v>
+      </c>
+      <c r="FA2" t="s">
+        <v>576</v>
+      </c>
+      <c r="FB2" t="s">
+        <v>575</v>
+      </c>
+      <c r="FC2" t="s">
+        <v>538</v>
+      </c>
+      <c r="FD2" t="s">
+        <v>577</v>
+      </c>
+      <c r="FE2" t="s">
+        <v>578</v>
+      </c>
+      <c r="FF2" t="s">
+        <v>545</v>
+      </c>
+      <c r="FG2" t="s">
+        <v>572</v>
+      </c>
+      <c r="FH2" t="s">
+        <v>579</v>
+      </c>
+      <c r="FI2" t="s">
+        <v>580</v>
+      </c>
+      <c r="FJ2" t="s">
+        <v>576</v>
+      </c>
+      <c r="FK2" t="s">
+        <v>581</v>
+      </c>
+      <c r="FL2" t="s">
+        <v>582</v>
+      </c>
+      <c r="FM2" t="s">
+        <v>572</v>
+      </c>
+      <c r="FN2" t="s">
+        <v>583</v>
+      </c>
+      <c r="FO2" t="s">
+        <v>541</v>
+      </c>
+      <c r="FP2" t="s">
+        <v>584</v>
+      </c>
+      <c r="FQ2" t="s">
+        <v>575</v>
+      </c>
+      <c r="FR2" t="s">
+        <v>580</v>
+      </c>
+      <c r="FS2" t="s">
+        <v>572</v>
+      </c>
+      <c r="FT2" t="s">
+        <v>585</v>
+      </c>
+      <c r="FU2" t="s">
+        <v>580</v>
+      </c>
+      <c r="FV2" t="s">
+        <v>576</v>
+      </c>
+      <c r="FW2" t="s">
+        <v>586</v>
+      </c>
+      <c r="FX2" t="s">
+        <v>582</v>
+      </c>
+      <c r="FY2" t="s">
+        <v>572</v>
+      </c>
+      <c r="FZ2" t="s">
+        <v>587</v>
+      </c>
+      <c r="GA2" t="s">
+        <v>580</v>
+      </c>
+      <c r="GB2" t="s">
+        <v>577</v>
+      </c>
+      <c r="GC2" t="s">
+        <v>588</v>
+      </c>
+      <c r="GD2" t="s">
+        <v>589</v>
+      </c>
+      <c r="GE2" t="s">
+        <v>577</v>
+      </c>
+      <c r="GF2" t="s">
+        <v>590</v>
+      </c>
+      <c r="GG2" t="s">
+        <v>589</v>
+      </c>
+      <c r="GH2" t="s">
+        <v>572</v>
+      </c>
+      <c r="GI2" t="s">
+        <v>591</v>
+      </c>
+      <c r="GJ2" t="s">
+        <v>592</v>
+      </c>
+      <c r="GK2" t="s">
+        <v>572</v>
+      </c>
+      <c r="GL2" t="s">
+        <v>590</v>
+      </c>
+      <c r="GM2" t="s">
+        <v>593</v>
+      </c>
+      <c r="GN2" t="s">
+        <v>576</v>
+      </c>
+      <c r="GO2" t="s">
+        <v>590</v>
+      </c>
+      <c r="GP2" t="s">
+        <v>594</v>
+      </c>
+      <c r="GQ2" t="s">
+        <v>572</v>
+      </c>
+      <c r="GR2" t="s">
+        <v>590</v>
+      </c>
+      <c r="GS2" t="s">
+        <v>593</v>
+      </c>
+      <c r="GT2" t="s">
+        <v>576</v>
+      </c>
+      <c r="GU2" t="s">
+        <v>595</v>
+      </c>
+      <c r="GV2" t="s">
+        <v>596</v>
+      </c>
+      <c r="GW2" t="s">
+        <v>572</v>
+      </c>
+      <c r="GX2" t="s">
+        <v>597</v>
+      </c>
+      <c r="GY2" t="s">
+        <v>593</v>
+      </c>
+      <c r="GZ2" t="s">
+        <v>598</v>
+      </c>
+      <c r="HA2" t="s">
+        <v>525</v>
+      </c>
+      <c r="HB2" t="s">
+        <v>599</v>
+      </c>
+      <c r="HC2" t="s">
+        <v>600</v>
+      </c>
+      <c r="HD2" t="s">
+        <v>601</v>
+      </c>
+      <c r="HE2" t="s">
+        <v>602</v>
+      </c>
+      <c r="HF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="HH2" t="s">
+        <v>526</v>
+      </c>
+      <c r="HI2" t="s">
+        <v>513</v>
+      </c>
+      <c r="HJ2" t="s">
+        <v>603</v>
+      </c>
+      <c r="HK2" t="s">
+        <v>604</v>
+      </c>
+      <c r="HL2" t="s">
+        <v>525</v>
+      </c>
+      <c r="HM2" t="s">
+        <v>513</v>
+      </c>
+      <c r="HN2" t="s">
+        <v>605</v>
+      </c>
+      <c r="HO2" t="s">
+        <v>606</v>
+      </c>
+      <c r="HP2" t="s">
+        <v>607</v>
+      </c>
+      <c r="HQ2" t="s">
+        <v>571</v>
+      </c>
+      <c r="HR2" t="s">
+        <v>608</v>
+      </c>
+      <c r="HS2" t="s">
+        <v>609</v>
+      </c>
+      <c r="HT2" t="s">
+        <v>521</v>
+      </c>
+      <c r="HU2" t="s">
+        <v>610</v>
+      </c>
+      <c r="HV2" t="s">
+        <v>604</v>
+      </c>
+      <c r="HW2" t="s">
+        <v>611</v>
+      </c>
+      <c r="HX2" t="s">
+        <v>612</v>
+      </c>
+      <c r="HY2" t="s">
+        <v>525</v>
+      </c>
+      <c r="HZ2" t="s">
+        <v>610</v>
+      </c>
+      <c r="IA2" t="s">
+        <v>604</v>
+      </c>
+      <c r="IB2" t="s">
+        <v>613</v>
+      </c>
+      <c r="IC2" t="s">
+        <v>614</v>
+      </c>
+      <c r="ID2" t="s">
+        <v>570</v>
+      </c>
+      <c r="IE2" t="s">
+        <v>610</v>
+      </c>
+      <c r="IF2" t="s">
+        <v>604</v>
+      </c>
+      <c r="IG2" t="s">
+        <v>615</v>
+      </c>
+      <c r="IH2" t="s">
+        <v>521</v>
+      </c>
+      <c r="II2" t="s">
+        <v>616</v>
+      </c>
+      <c r="IJ2" t="s">
+        <v>617</v>
+      </c>
+      <c r="IK2" t="s">
+        <v>618</v>
+      </c>
+      <c r="IL2" t="s">
+        <v>619</v>
+      </c>
+      <c r="IM2" t="s">
+        <v>527</v>
+      </c>
+      <c r="IN2" t="s">
+        <v>620</v>
+      </c>
+      <c r="IO2" t="s">
+        <v>621</v>
+      </c>
+      <c r="IP2" t="s">
+        <v>622</v>
+      </c>
+      <c r="IQ2" t="s">
+        <v>623</v>
+      </c>
+      <c r="IR2" t="s">
+        <v>624</v>
+      </c>
+      <c r="IS2" t="s">
+        <v>625</v>
+      </c>
+      <c r="IT2" t="s">
+        <v>626</v>
+      </c>
+      <c r="IU2" t="s">
+        <v>627</v>
+      </c>
+      <c r="IV2" t="s">
+        <v>628</v>
+      </c>
+      <c r="IW2" t="s">
+        <v>513</v>
+      </c>
+      <c r="IX2" t="s">
+        <v>629</v>
+      </c>
+      <c r="IY2" t="s">
+        <v>630</v>
+      </c>
+      <c r="IZ2" t="s">
+        <v>631</v>
+      </c>
+      <c r="JA2" t="s">
+        <v>628</v>
+      </c>
+      <c r="JB2" t="s">
+        <v>632</v>
+      </c>
+      <c r="JC2" t="s">
+        <v>633</v>
+      </c>
+      <c r="JD2" t="s">
+        <v>634</v>
+      </c>
+      <c r="JE2" t="s">
+        <v>635</v>
+      </c>
+      <c r="JF2" t="s">
+        <v>525</v>
+      </c>
+      <c r="JG2" t="s">
+        <v>521</v>
+      </c>
+      <c r="JH2" t="s">
+        <v>612</v>
+      </c>
+      <c r="JI2" t="s">
+        <v>636</v>
+      </c>
+      <c r="JJ2" t="s">
+        <v>637</v>
+      </c>
+      <c r="JK2" t="s">
+        <v>610</v>
+      </c>
+      <c r="JL2" t="s">
+        <v>610</v>
+      </c>
+      <c r="JM2" t="s">
+        <v>569</v>
+      </c>
+      <c r="JN2" t="s">
+        <v>610</v>
+      </c>
+      <c r="JO2" t="s">
+        <v>638</v>
+      </c>
+      <c r="JP2" t="s">
+        <v>525</v>
+      </c>
+      <c r="JQ2" t="s">
+        <v>520</v>
+      </c>
+      <c r="JR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="JZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KA2" t="s">
+        <v>525</v>
+      </c>
+      <c r="KB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KK2" t="s">
+        <v>639</v>
+      </c>
+      <c r="KL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="KM2" t="s">
+        <v>640</v>
+      </c>
+      <c r="KN2" t="s">
         <v>522</v>
       </c>
-      <c r="AL2" t="s">
-        <v>533</v>
-      </c>
-      <c r="AM2" t="s">
+      <c r="KO2" t="s">
+        <v>610</v>
+      </c>
+      <c r="KP2" t="s">
         <v>522</v>
       </c>
-      <c r="AN2" t="s">
-        <v>534</v>
-      </c>
-      <c r="AO2" t="s">
+      <c r="KQ2" t="s">
+        <v>641</v>
+      </c>
+      <c r="KR2" t="s">
         <v>522</v>
       </c>
-      <c r="AP2" t="s">
-        <v>533</v>
-      </c>
-      <c r="AQ2" t="s">
+      <c r="KS2" t="s">
+        <v>610</v>
+      </c>
+      <c r="KT2" t="s">
+        <v>522</v>
+      </c>
+      <c r="KU2" t="s">
+        <v>640</v>
+      </c>
+      <c r="KV2" t="s">
+        <v>522</v>
+      </c>
+      <c r="KW2" t="s">
+        <v>610</v>
+      </c>
+      <c r="KX2" t="s">
+        <v>522</v>
+      </c>
+      <c r="KY2" t="s">
+        <v>642</v>
+      </c>
+      <c r="KZ2" t="s">
+        <v>522</v>
+      </c>
+      <c r="LA2" t="s">
+        <v>610</v>
+      </c>
+      <c r="LB2" t="s">
+        <v>522</v>
+      </c>
+      <c r="LC2" t="s">
+        <v>522</v>
+      </c>
+      <c r="LD2" t="s">
+        <v>522</v>
+      </c>
+      <c r="LE2" t="s">
+        <v>643</v>
+      </c>
+      <c r="LF2" t="s">
+        <v>644</v>
+      </c>
+      <c r="LG2" t="s">
+        <v>645</v>
+      </c>
+      <c r="LH2" t="s">
+        <v>646</v>
+      </c>
+      <c r="LI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="LZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="MD2" t="s">
         <v>518</v>
       </c>
-      <c r="AR2" t="s">
-        <v>137</v>
-      </c>
-      <c r="AS2" t="s">
+      <c r="ME2" t="s">
+        <v>526</v>
+      </c>
+      <c r="MF2" t="s">
+        <v>647</v>
+      </c>
+      <c r="MG2" t="s">
+        <v>527</v>
+      </c>
+      <c r="MH2" t="s">
+        <v>518</v>
+      </c>
+      <c r="MI2" t="s">
+        <v>569</v>
+      </c>
+      <c r="MJ2" t="s">
+        <v>648</v>
+      </c>
+      <c r="MK2" t="s">
+        <v>571</v>
+      </c>
+      <c r="ML2" t="s">
+        <v>649</v>
+      </c>
+      <c r="MM2" t="s">
+        <v>570</v>
+      </c>
+      <c r="MN2" t="s">
+        <v>608</v>
+      </c>
+      <c r="MO2" t="s">
+        <v>609</v>
+      </c>
+      <c r="MP2" t="s">
+        <v>521</v>
+      </c>
+      <c r="MQ2" t="s">
+        <v>610</v>
+      </c>
+      <c r="MR2" t="s">
+        <v>604</v>
+      </c>
+      <c r="MS2" t="s">
+        <v>611</v>
+      </c>
+      <c r="MT2" t="s">
+        <v>612</v>
+      </c>
+      <c r="MU2" t="s">
+        <v>525</v>
+      </c>
+      <c r="MV2" t="s">
+        <v>610</v>
+      </c>
+      <c r="MW2" t="s">
+        <v>604</v>
+      </c>
+      <c r="MX2" t="s">
+        <v>613</v>
+      </c>
+      <c r="MY2" t="s">
+        <v>614</v>
+      </c>
+      <c r="MZ2" t="s">
+        <v>570</v>
+      </c>
+      <c r="NA2" t="s">
+        <v>610</v>
+      </c>
+      <c r="NB2" t="s">
+        <v>604</v>
+      </c>
+      <c r="NC2" t="s">
+        <v>615</v>
+      </c>
+      <c r="ND2" t="s">
+        <v>521</v>
+      </c>
+      <c r="NE2" t="s">
+        <v>616</v>
+      </c>
+      <c r="NF2" t="s">
+        <v>617</v>
+      </c>
+      <c r="NG2" t="s">
+        <v>618</v>
+      </c>
+      <c r="NH2" t="s">
+        <v>619</v>
+      </c>
+      <c r="NI2" t="s">
+        <v>527</v>
+      </c>
+      <c r="NJ2" t="s">
+        <v>620</v>
+      </c>
+      <c r="NK2" t="s">
+        <v>621</v>
+      </c>
+      <c r="NL2" t="s">
+        <v>622</v>
+      </c>
+      <c r="NM2" t="s">
+        <v>623</v>
+      </c>
+      <c r="NN2" t="s">
+        <v>624</v>
+      </c>
+      <c r="NO2" t="s">
+        <v>625</v>
+      </c>
+      <c r="NP2" t="s">
+        <v>626</v>
+      </c>
+      <c r="NQ2" t="s">
+        <v>627</v>
+      </c>
+      <c r="NR2" t="s">
+        <v>628</v>
+      </c>
+      <c r="NS2" t="s">
+        <v>513</v>
+      </c>
+      <c r="NT2" t="s">
+        <v>629</v>
+      </c>
+      <c r="NU2" t="s">
+        <v>630</v>
+      </c>
+      <c r="NV2" t="s">
+        <v>631</v>
+      </c>
+      <c r="NW2" t="s">
+        <v>628</v>
+      </c>
+      <c r="NX2" t="s">
+        <v>632</v>
+      </c>
+      <c r="NY2" t="s">
+        <v>633</v>
+      </c>
+      <c r="NZ2" t="s">
+        <v>634</v>
+      </c>
+      <c r="OA2" t="s">
+        <v>635</v>
+      </c>
+      <c r="OB2" t="s">
+        <v>525</v>
+      </c>
+      <c r="OC2" t="s">
+        <v>521</v>
+      </c>
+      <c r="OD2" t="s">
+        <v>612</v>
+      </c>
+      <c r="OE2" t="s">
+        <v>636</v>
+      </c>
+      <c r="OF2" t="s">
+        <v>650</v>
+      </c>
+      <c r="OG2" t="s">
+        <v>513</v>
+      </c>
+      <c r="OH2" t="s">
+        <v>651</v>
+      </c>
+      <c r="OI2" t="s">
+        <v>571</v>
+      </c>
+      <c r="OJ2" t="s">
+        <v>518</v>
+      </c>
+      <c r="OK2" t="s">
+        <v>652</v>
+      </c>
+      <c r="OL2" t="s">
+        <v>569</v>
+      </c>
+      <c r="OM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ON2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="OZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="PI2" t="s">
+        <v>653</v>
+      </c>
+      <c r="PJ2" t="s">
+        <v>520</v>
+      </c>
+      <c r="PK2" t="s">
+        <v>610</v>
+      </c>
+      <c r="PL2" t="s">
+        <v>520</v>
+      </c>
+      <c r="PM2" t="s">
+        <v>653</v>
+      </c>
+      <c r="PN2" t="s">
+        <v>520</v>
+      </c>
+      <c r="PO2" t="s">
+        <v>610</v>
+      </c>
+      <c r="PP2" t="s">
+        <v>520</v>
+      </c>
+      <c r="PQ2" t="s">
+        <v>653</v>
+      </c>
+      <c r="PR2" t="s">
+        <v>520</v>
+      </c>
+      <c r="PS2" t="s">
+        <v>610</v>
+      </c>
+      <c r="PT2" t="s">
+        <v>520</v>
+      </c>
+      <c r="PU2" t="s">
+        <v>653</v>
+      </c>
+      <c r="PV2" t="s">
+        <v>520</v>
+      </c>
+      <c r="PW2" t="s">
+        <v>610</v>
+      </c>
+      <c r="PX2" t="s">
+        <v>520</v>
+      </c>
+      <c r="PY2" t="s">
+        <v>520</v>
+      </c>
+      <c r="PZ2" t="s">
+        <v>520</v>
+      </c>
+      <c r="QA2" t="s">
+        <v>654</v>
+      </c>
+      <c r="QB2" t="s">
+        <v>654</v>
+      </c>
+      <c r="QC2" t="s">
+        <v>654</v>
+      </c>
+      <c r="QD2" t="s">
+        <v>654</v>
+      </c>
+      <c r="QE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="QX2" t="s">
+        <v>518</v>
+      </c>
+      <c r="QY2" t="s">
+        <v>526</v>
+      </c>
+      <c r="QZ2" t="s">
+        <v>647</v>
+      </c>
+      <c r="RA2" t="s">
+        <v>527</v>
+      </c>
+      <c r="RB2" t="s">
+        <v>610</v>
+      </c>
+      <c r="RC2" t="s">
+        <v>610</v>
+      </c>
+      <c r="RD2" t="s">
+        <v>610</v>
+      </c>
+      <c r="RE2" t="s">
+        <v>610</v>
+      </c>
+      <c r="RF2" t="s">
         <v>522</v>
       </c>
-      <c r="AT2" t="s">
-        <v>535</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>522</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>536</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>522</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>535</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>522</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>535</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>522</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>537</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>522</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>538</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>522</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>538</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>522</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>535</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>522</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>533</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>522</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>539</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>522</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>535</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>522</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>535</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>522</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>540</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>522</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>539</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>522</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>541</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>518</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>137</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>522</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>518</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>518</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>522</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>522</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>518</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>522</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>542</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>522</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>538</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>518</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>522</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>543</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>518</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>522</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>539</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>518</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>137</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>522</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>544</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>522</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>539</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>522</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>540</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>522</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>544</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>518</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>518</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>518</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>137</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>545</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>546</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>547</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>548</v>
-      </c>
-      <c r="DQ2" t="s">
-        <v>549</v>
-      </c>
-      <c r="DR2" t="s">
-        <v>550</v>
-      </c>
-      <c r="DS2" t="s">
-        <v>551</v>
-      </c>
-      <c r="DT2" t="s">
-        <v>552</v>
-      </c>
-      <c r="DU2" t="s">
-        <v>553</v>
-      </c>
-      <c r="DV2" t="s">
-        <v>554</v>
-      </c>
-      <c r="DW2" t="s">
-        <v>555</v>
-      </c>
-      <c r="DX2" t="s">
-        <v>556</v>
-      </c>
-      <c r="DY2" t="s">
-        <v>557</v>
-      </c>
-      <c r="DZ2" t="s">
-        <v>558</v>
-      </c>
-      <c r="EA2" t="s">
-        <v>559</v>
-      </c>
-      <c r="EB2" t="s">
-        <v>560</v>
-      </c>
-      <c r="EC2" t="s">
-        <v>561</v>
-      </c>
-      <c r="ED2" t="s">
-        <v>562</v>
-      </c>
-      <c r="EE2" t="s">
-        <v>563</v>
-      </c>
-      <c r="EF2" t="s">
-        <v>564</v>
-      </c>
-      <c r="EG2" t="s">
-        <v>565</v>
-      </c>
-      <c r="EH2" t="s">
-        <v>566</v>
-      </c>
-      <c r="EI2" t="s">
-        <v>567</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>519</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>520</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>521</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>517</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>524</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>525</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>526</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>568</v>
-      </c>
-      <c r="ER2" t="s">
-        <v>569</v>
-      </c>
-      <c r="ES2" t="s">
-        <v>512</v>
-      </c>
-      <c r="ET2" t="s">
-        <v>570</v>
-      </c>
-      <c r="EU2" t="s">
-        <v>571</v>
-      </c>
-      <c r="EV2" t="s">
-        <v>572</v>
-      </c>
-      <c r="EW2" t="s">
-        <v>573</v>
-      </c>
-      <c r="EX2" t="s">
-        <v>571</v>
-      </c>
-      <c r="EY2" t="s">
-        <v>574</v>
-      </c>
-      <c r="EZ2" t="s">
-        <v>539</v>
-      </c>
-      <c r="FA2" t="s">
-        <v>575</v>
-      </c>
-      <c r="FB2" t="s">
-        <v>574</v>
-      </c>
-      <c r="FC2" t="s">
-        <v>537</v>
-      </c>
-      <c r="FD2" t="s">
-        <v>576</v>
-      </c>
-      <c r="FE2" t="s">
-        <v>577</v>
-      </c>
-      <c r="FF2" t="s">
-        <v>544</v>
-      </c>
-      <c r="FG2" t="s">
-        <v>571</v>
-      </c>
-      <c r="FH2" t="s">
-        <v>578</v>
-      </c>
-      <c r="FI2" t="s">
-        <v>579</v>
-      </c>
-      <c r="FJ2" t="s">
-        <v>575</v>
-      </c>
-      <c r="FK2" t="s">
-        <v>580</v>
-      </c>
-      <c r="FL2" t="s">
-        <v>581</v>
-      </c>
-      <c r="FM2" t="s">
-        <v>571</v>
-      </c>
-      <c r="FN2" t="s">
-        <v>582</v>
-      </c>
-      <c r="FO2" t="s">
-        <v>540</v>
-      </c>
-      <c r="FP2" t="s">
-        <v>583</v>
-      </c>
-      <c r="FQ2" t="s">
-        <v>574</v>
-      </c>
-      <c r="FR2" t="s">
-        <v>579</v>
-      </c>
-      <c r="FS2" t="s">
-        <v>571</v>
-      </c>
-      <c r="FT2" t="s">
-        <v>584</v>
-      </c>
-      <c r="FU2" t="s">
-        <v>579</v>
-      </c>
-      <c r="FV2" t="s">
-        <v>575</v>
-      </c>
-      <c r="FW2" t="s">
-        <v>585</v>
-      </c>
-      <c r="FX2" t="s">
-        <v>581</v>
-      </c>
-      <c r="FY2" t="s">
-        <v>571</v>
-      </c>
-      <c r="FZ2" t="s">
-        <v>586</v>
-      </c>
-      <c r="GA2" t="s">
-        <v>579</v>
-      </c>
-      <c r="GB2" t="s">
-        <v>576</v>
-      </c>
-      <c r="GC2" t="s">
-        <v>587</v>
-      </c>
-      <c r="GD2" t="s">
-        <v>588</v>
-      </c>
-      <c r="GE2" t="s">
-        <v>576</v>
-      </c>
-      <c r="GF2" t="s">
-        <v>589</v>
-      </c>
-      <c r="GG2" t="s">
-        <v>588</v>
-      </c>
-      <c r="GH2" t="s">
-        <v>571</v>
-      </c>
-      <c r="GI2" t="s">
-        <v>590</v>
-      </c>
-      <c r="GJ2" t="s">
-        <v>591</v>
-      </c>
-      <c r="GK2" t="s">
-        <v>571</v>
-      </c>
-      <c r="GL2" t="s">
-        <v>589</v>
-      </c>
-      <c r="GM2" t="s">
-        <v>592</v>
-      </c>
-      <c r="GN2" t="s">
-        <v>575</v>
-      </c>
-      <c r="GO2" t="s">
-        <v>589</v>
-      </c>
-      <c r="GP2" t="s">
-        <v>593</v>
-      </c>
-      <c r="GQ2" t="s">
-        <v>571</v>
-      </c>
-      <c r="GR2" t="s">
-        <v>589</v>
-      </c>
-      <c r="GS2" t="s">
-        <v>592</v>
-      </c>
-      <c r="GT2" t="s">
-        <v>575</v>
-      </c>
-      <c r="GU2" t="s">
-        <v>594</v>
-      </c>
-      <c r="GV2" t="s">
-        <v>595</v>
-      </c>
-      <c r="GW2" t="s">
-        <v>571</v>
-      </c>
-      <c r="GX2" t="s">
-        <v>596</v>
-      </c>
-      <c r="GY2" t="s">
-        <v>592</v>
-      </c>
-      <c r="GZ2" t="s">
-        <v>597</v>
-      </c>
-      <c r="HA2" t="s">
-        <v>524</v>
-      </c>
-      <c r="HB2" t="s">
-        <v>598</v>
-      </c>
-      <c r="HC2" t="s">
-        <v>599</v>
-      </c>
-      <c r="HD2" t="s">
-        <v>600</v>
-      </c>
-      <c r="HE2" t="s">
-        <v>601</v>
-      </c>
-      <c r="HF2" t="s">
-        <v>137</v>
-      </c>
-      <c r="HG2" t="s">
-        <v>137</v>
-      </c>
-      <c r="HH2" t="s">
-        <v>525</v>
-      </c>
-      <c r="HI2" t="s">
-        <v>512</v>
-      </c>
-      <c r="HJ2" t="s">
-        <v>602</v>
-      </c>
-      <c r="HK2" t="s">
-        <v>603</v>
-      </c>
-      <c r="HL2" t="s">
-        <v>524</v>
-      </c>
-      <c r="HM2" t="s">
-        <v>512</v>
-      </c>
-      <c r="HN2" t="s">
-        <v>604</v>
-      </c>
-      <c r="HO2" t="s">
-        <v>605</v>
-      </c>
-      <c r="HP2" t="s">
-        <v>606</v>
-      </c>
-      <c r="HQ2" t="s">
-        <v>570</v>
-      </c>
-      <c r="HR2" t="s">
-        <v>607</v>
-      </c>
-      <c r="HS2" t="s">
-        <v>608</v>
-      </c>
-      <c r="HT2" t="s">
-        <v>520</v>
-      </c>
-      <c r="HU2" t="s">
-        <v>609</v>
-      </c>
-      <c r="HV2" t="s">
-        <v>603</v>
-      </c>
-      <c r="HW2" t="s">
+      <c r="RG2" t="s">
         <v>610</v>
       </c>
-      <c r="HX2" t="s">
-        <v>611</v>
-      </c>
-      <c r="HY2" t="s">
-        <v>524</v>
-      </c>
-      <c r="HZ2" t="s">
-        <v>609</v>
-      </c>
-      <c r="IA2" t="s">
-        <v>603</v>
-      </c>
-      <c r="IB2" t="s">
-        <v>612</v>
-      </c>
-      <c r="IC2" t="s">
-        <v>613</v>
-      </c>
-      <c r="ID2" t="s">
-        <v>569</v>
-      </c>
-      <c r="IE2" t="s">
-        <v>609</v>
-      </c>
-      <c r="IF2" t="s">
-        <v>603</v>
-      </c>
-      <c r="IG2" t="s">
-        <v>614</v>
-      </c>
-      <c r="IH2" t="s">
-        <v>520</v>
-      </c>
-      <c r="II2" t="s">
-        <v>615</v>
-      </c>
-      <c r="IJ2" t="s">
-        <v>616</v>
-      </c>
-      <c r="IK2" t="s">
-        <v>617</v>
-      </c>
-      <c r="IL2" t="s">
-        <v>618</v>
-      </c>
-      <c r="IM2" t="s">
-        <v>526</v>
-      </c>
-      <c r="IN2" t="s">
-        <v>619</v>
-      </c>
-      <c r="IO2" t="s">
-        <v>620</v>
-      </c>
-      <c r="IP2" t="s">
-        <v>621</v>
-      </c>
-      <c r="IQ2" t="s">
-        <v>622</v>
-      </c>
-      <c r="IR2" t="s">
-        <v>623</v>
-      </c>
-      <c r="IS2" t="s">
-        <v>624</v>
-      </c>
-      <c r="IT2" t="s">
-        <v>625</v>
-      </c>
-      <c r="IU2" t="s">
-        <v>626</v>
-      </c>
-      <c r="IV2" t="s">
-        <v>627</v>
-      </c>
-      <c r="IW2" t="s">
-        <v>512</v>
-      </c>
-      <c r="IX2" t="s">
-        <v>628</v>
-      </c>
-      <c r="IY2" t="s">
-        <v>629</v>
-      </c>
-      <c r="IZ2" t="s">
-        <v>630</v>
-      </c>
-      <c r="JA2" t="s">
-        <v>627</v>
-      </c>
-      <c r="JB2" t="s">
-        <v>631</v>
-      </c>
-      <c r="JC2" t="s">
-        <v>632</v>
-      </c>
-      <c r="JD2" t="s">
-        <v>633</v>
-      </c>
-      <c r="JE2" t="s">
-        <v>634</v>
-      </c>
-      <c r="JF2" t="s">
-        <v>524</v>
-      </c>
-      <c r="JG2" t="s">
-        <v>520</v>
-      </c>
-      <c r="JH2" t="s">
-        <v>611</v>
-      </c>
-      <c r="JI2" t="s">
-        <v>635</v>
-      </c>
-      <c r="JJ2" t="s">
-        <v>636</v>
-      </c>
-      <c r="JK2" t="s">
-        <v>609</v>
-      </c>
-      <c r="JL2" t="s">
-        <v>609</v>
-      </c>
-      <c r="JM2" t="s">
-        <v>568</v>
-      </c>
-      <c r="JN2" t="s">
-        <v>609</v>
-      </c>
-      <c r="JO2" t="s">
-        <v>637</v>
-      </c>
-      <c r="JP2" t="s">
-        <v>524</v>
-      </c>
-      <c r="JQ2" t="s">
-        <v>519</v>
-      </c>
-      <c r="JR2" t="s">
-        <v>137</v>
-      </c>
-      <c r="JS2" t="s">
-        <v>137</v>
-      </c>
-      <c r="JT2" t="s">
-        <v>137</v>
-      </c>
-      <c r="JU2" t="s">
-        <v>137</v>
-      </c>
-      <c r="JV2" t="s">
-        <v>137</v>
-      </c>
-      <c r="JW2" t="s">
-        <v>137</v>
-      </c>
-      <c r="JX2" t="s">
-        <v>137</v>
-      </c>
-      <c r="JY2" t="s">
-        <v>137</v>
-      </c>
-      <c r="JZ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KA2" t="s">
-        <v>524</v>
-      </c>
-      <c r="KB2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KC2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KD2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KE2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KF2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KG2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KI2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KJ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KK2" t="s">
-        <v>638</v>
-      </c>
-      <c r="KL2" t="s">
-        <v>137</v>
-      </c>
-      <c r="KM2" t="s">
-        <v>639</v>
-      </c>
-      <c r="KN2" t="s">
-        <v>521</v>
-      </c>
-      <c r="KO2" t="s">
-        <v>609</v>
-      </c>
-      <c r="KP2" t="s">
-        <v>521</v>
-      </c>
-      <c r="KQ2" t="s">
-        <v>640</v>
-      </c>
-      <c r="KR2" t="s">
-        <v>521</v>
-      </c>
-      <c r="KS2" t="s">
-        <v>609</v>
-      </c>
-      <c r="KT2" t="s">
-        <v>521</v>
-      </c>
-      <c r="KU2" t="s">
-        <v>639</v>
-      </c>
-      <c r="KV2" t="s">
-        <v>521</v>
-      </c>
-      <c r="KW2" t="s">
-        <v>609</v>
-      </c>
-      <c r="KX2" t="s">
-        <v>521</v>
-      </c>
-      <c r="KY2" t="s">
-        <v>641</v>
-      </c>
-      <c r="KZ2" t="s">
-        <v>521</v>
-      </c>
-      <c r="LA2" t="s">
-        <v>609</v>
-      </c>
-      <c r="LB2" t="s">
-        <v>521</v>
-      </c>
-      <c r="LC2" t="s">
-        <v>521</v>
-      </c>
-      <c r="LD2" t="s">
-        <v>521</v>
-      </c>
-      <c r="LE2" t="s">
-        <v>642</v>
-      </c>
-      <c r="LF2" t="s">
-        <v>643</v>
-      </c>
-      <c r="LG2" t="s">
-        <v>644</v>
-      </c>
-      <c r="LH2" t="s">
-        <v>645</v>
-      </c>
-      <c r="LI2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LJ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LK2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LL2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LM2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LN2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LO2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LP2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LQ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LR2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LS2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LT2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LU2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LV2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LW2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LX2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LY2" t="s">
-        <v>137</v>
-      </c>
-      <c r="LZ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="MA2" t="s">
-        <v>137</v>
-      </c>
-      <c r="MB2" t="s">
-        <v>137</v>
-      </c>
-      <c r="MC2" t="s">
-        <v>137</v>
-      </c>
-      <c r="MD2" t="s">
-        <v>517</v>
-      </c>
-      <c r="ME2" t="s">
-        <v>525</v>
-      </c>
-      <c r="MF2" t="s">
-        <v>646</v>
-      </c>
-      <c r="MG2" t="s">
-        <v>526</v>
-      </c>
-      <c r="MH2" t="s">
-        <v>517</v>
-      </c>
-      <c r="MI2" t="s">
-        <v>568</v>
-      </c>
-      <c r="MJ2" t="s">
-        <v>647</v>
-      </c>
-      <c r="MK2" t="s">
-        <v>570</v>
-      </c>
-      <c r="ML2" t="s">
-        <v>648</v>
-      </c>
-      <c r="MM2" t="s">
-        <v>569</v>
-      </c>
-      <c r="MN2" t="s">
-        <v>607</v>
-      </c>
-      <c r="MO2" t="s">
-        <v>608</v>
-      </c>
-      <c r="MP2" t="s">
-        <v>520</v>
-      </c>
-      <c r="MQ2" t="s">
-        <v>609</v>
-      </c>
-      <c r="MR2" t="s">
-        <v>603</v>
-      </c>
-      <c r="MS2" t="s">
+      <c r="RH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="RZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SC2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SE2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="ST2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="SZ2" t="s">
         <v>610</v>
       </c>
-      <c r="MT2" t="s">
-        <v>611</v>
-      </c>
-      <c r="MU2" t="s">
-        <v>524</v>
-      </c>
-      <c r="MV2" t="s">
-        <v>609</v>
-      </c>
-      <c r="MW2" t="s">
-        <v>603</v>
-      </c>
-      <c r="MX2" t="s">
-        <v>612</v>
-      </c>
-      <c r="MY2" t="s">
-        <v>613</v>
-      </c>
-      <c r="MZ2" t="s">
-        <v>569</v>
-      </c>
-      <c r="NA2" t="s">
-        <v>609</v>
-      </c>
-      <c r="NB2" t="s">
-        <v>603</v>
-      </c>
-      <c r="NC2" t="s">
-        <v>614</v>
-      </c>
-      <c r="ND2" t="s">
-        <v>520</v>
-      </c>
-      <c r="NE2" t="s">
-        <v>615</v>
-      </c>
-      <c r="NF2" t="s">
-        <v>616</v>
-      </c>
-      <c r="NG2" t="s">
-        <v>617</v>
-      </c>
-      <c r="NH2" t="s">
-        <v>618</v>
-      </c>
-      <c r="NI2" t="s">
-        <v>526</v>
-      </c>
-      <c r="NJ2" t="s">
-        <v>619</v>
-      </c>
-      <c r="NK2" t="s">
-        <v>620</v>
-      </c>
-      <c r="NL2" t="s">
-        <v>621</v>
-      </c>
-      <c r="NM2" t="s">
-        <v>622</v>
-      </c>
-      <c r="NN2" t="s">
-        <v>623</v>
-      </c>
-      <c r="NO2" t="s">
-        <v>624</v>
-      </c>
-      <c r="NP2" t="s">
-        <v>625</v>
-      </c>
-      <c r="NQ2" t="s">
-        <v>626</v>
-      </c>
-      <c r="NR2" t="s">
-        <v>627</v>
-      </c>
-      <c r="NS2" t="s">
-        <v>512</v>
-      </c>
-      <c r="NT2" t="s">
-        <v>628</v>
-      </c>
-      <c r="NU2" t="s">
-        <v>629</v>
-      </c>
-      <c r="NV2" t="s">
-        <v>630</v>
-      </c>
-      <c r="NW2" t="s">
-        <v>627</v>
-      </c>
-      <c r="NX2" t="s">
-        <v>631</v>
-      </c>
-      <c r="NY2" t="s">
-        <v>632</v>
-      </c>
-      <c r="NZ2" t="s">
-        <v>633</v>
-      </c>
-      <c r="OA2" t="s">
-        <v>634</v>
-      </c>
-      <c r="OB2" t="s">
-        <v>524</v>
-      </c>
-      <c r="OC2" t="s">
-        <v>520</v>
-      </c>
-      <c r="OD2" t="s">
-        <v>611</v>
-      </c>
-      <c r="OE2" t="s">
-        <v>635</v>
-      </c>
-      <c r="OF2" t="s">
-        <v>649</v>
-      </c>
-      <c r="OG2" t="s">
-        <v>512</v>
-      </c>
-      <c r="OH2" t="s">
-        <v>650</v>
-      </c>
-      <c r="OI2" t="s">
-        <v>570</v>
-      </c>
-      <c r="OJ2" t="s">
-        <v>517</v>
-      </c>
-      <c r="OK2" t="s">
-        <v>651</v>
-      </c>
-      <c r="OL2" t="s">
-        <v>568</v>
-      </c>
-      <c r="OM2" t="s">
-        <v>137</v>
-      </c>
-      <c r="ON2" t="s">
-        <v>137</v>
-      </c>
-      <c r="OO2" t="s">
-        <v>137</v>
-      </c>
-      <c r="OP2" t="s">
-        <v>137</v>
-      </c>
-      <c r="OQ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="OR2" t="s">
-        <v>137</v>
-      </c>
-      <c r="OS2" t="s">
-        <v>137</v>
-      </c>
-      <c r="OT2" t="s">
-        <v>137</v>
-      </c>
-      <c r="OU2" t="s">
-        <v>137</v>
-      </c>
-      <c r="OV2" t="s">
-        <v>137</v>
-      </c>
-      <c r="OW2" t="s">
-        <v>137</v>
-      </c>
-      <c r="OX2" t="s">
-        <v>137</v>
-      </c>
-      <c r="OY2" t="s">
-        <v>137</v>
-      </c>
-      <c r="OZ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="PA2" t="s">
-        <v>137</v>
-      </c>
-      <c r="PB2" t="s">
-        <v>137</v>
-      </c>
-      <c r="PC2" t="s">
-        <v>137</v>
-      </c>
-      <c r="PD2" t="s">
-        <v>137</v>
-      </c>
-      <c r="PE2" t="s">
-        <v>137</v>
-      </c>
-      <c r="PF2" t="s">
-        <v>137</v>
-      </c>
-      <c r="PG2" t="s">
-        <v>137</v>
-      </c>
-      <c r="PH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="PI2" t="s">
-        <v>652</v>
-      </c>
-      <c r="PJ2" t="s">
-        <v>519</v>
-      </c>
-      <c r="PK2" t="s">
-        <v>609</v>
-      </c>
-      <c r="PL2" t="s">
-        <v>519</v>
-      </c>
-      <c r="PM2" t="s">
-        <v>652</v>
-      </c>
-      <c r="PN2" t="s">
-        <v>519</v>
-      </c>
-      <c r="PO2" t="s">
-        <v>609</v>
-      </c>
-      <c r="PP2" t="s">
-        <v>519</v>
-      </c>
-      <c r="PQ2" t="s">
-        <v>652</v>
-      </c>
-      <c r="PR2" t="s">
-        <v>519</v>
-      </c>
-      <c r="PS2" t="s">
-        <v>609</v>
-      </c>
-      <c r="PT2" t="s">
-        <v>519</v>
-      </c>
-      <c r="PU2" t="s">
-        <v>652</v>
-      </c>
-      <c r="PV2" t="s">
-        <v>519</v>
-      </c>
-      <c r="PW2" t="s">
-        <v>609</v>
-      </c>
-      <c r="PX2" t="s">
-        <v>519</v>
-      </c>
-      <c r="PY2" t="s">
-        <v>519</v>
-      </c>
-      <c r="PZ2" t="s">
-        <v>519</v>
-      </c>
-      <c r="QA2" t="s">
+      <c r="TA2" t="s">
+        <v>610</v>
+      </c>
+      <c r="TB2" t="s">
+        <v>610</v>
+      </c>
+      <c r="TC2" t="s">
+        <v>610</v>
+      </c>
+      <c r="TD2" t="s">
+        <v>610</v>
+      </c>
+      <c r="TE2" t="s">
+        <v>610</v>
+      </c>
+      <c r="TF2" t="s">
+        <v>610</v>
+      </c>
+      <c r="TG2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TI2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TK2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TM2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TO2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TP2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TQ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TR2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TS2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TT2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TU2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TV2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TW2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TX2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TY2" t="s">
+        <v>137</v>
+      </c>
+      <c r="TZ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UA2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UB2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UC2" t="s">
         <v>653</v>
       </c>
-      <c r="QB2" t="s">
+      <c r="UD2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UE2" t="s">
+        <v>610</v>
+      </c>
+      <c r="UF2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UG2" t="s">
         <v>653</v>
       </c>
-      <c r="QC2" t="s">
+      <c r="UH2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UI2" t="s">
+        <v>610</v>
+      </c>
+      <c r="UJ2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UK2" t="s">
         <v>653</v>
       </c>
-      <c r="QD2" t="s">
+      <c r="UL2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UM2" t="s">
+        <v>610</v>
+      </c>
+      <c r="UN2" t="s">
+        <v>137</v>
+      </c>
+      <c r="UO2" t="s">
         <v>653</v>
       </c>
-      <c r="QE2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QF2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QG2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QI2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QJ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QK2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QL2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QM2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QN2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QO2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QP2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QQ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QR2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QS2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QT2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QU2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QV2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QW2" t="s">
-        <v>137</v>
-      </c>
-      <c r="QX2" t="s">
-        <v>517</v>
-      </c>
-      <c r="QY2" t="s">
-        <v>525</v>
-      </c>
-      <c r="QZ2" t="s">
-        <v>646</v>
-      </c>
-      <c r="RA2" t="s">
-        <v>526</v>
-      </c>
-      <c r="RB2" t="s">
-        <v>609</v>
-      </c>
-      <c r="RC2" t="s">
-        <v>609</v>
-      </c>
-      <c r="RD2" t="s">
-        <v>609</v>
-      </c>
-      <c r="RE2" t="s">
-        <v>609</v>
-      </c>
-      <c r="RF2" t="s">
-        <v>521</v>
-      </c>
-      <c r="RG2" t="s">
-        <v>609</v>
-      </c>
-      <c r="RH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RI2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RJ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RK2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RL2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RM2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RN2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RO2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RP2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RQ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RR2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RS2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RT2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RU2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RV2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RW2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RX2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RY2" t="s">
-        <v>137</v>
-      </c>
-      <c r="RZ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SA2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SB2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SC2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SD2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SE2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SF2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SG2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SI2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SJ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SK2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SL2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SM2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SN2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SO2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SP2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SQ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SR2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SS2" t="s">
-        <v>137</v>
-      </c>
-      <c r="ST2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SU2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SV2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SW2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SX2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SY2" t="s">
-        <v>137</v>
-      </c>
-      <c r="SZ2" t="s">
-        <v>609</v>
-      </c>
-      <c r="TA2" t="s">
-        <v>609</v>
-      </c>
-      <c r="TB2" t="s">
-        <v>609</v>
-      </c>
-      <c r="TC2" t="s">
-        <v>609</v>
-      </c>
-      <c r="TD2" t="s">
-        <v>609</v>
-      </c>
-      <c r="TE2" t="s">
-        <v>609</v>
-      </c>
-      <c r="TF2" t="s">
-        <v>609</v>
-      </c>
-      <c r="TG2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TI2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TJ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TK2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TL2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TM2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TN2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TO2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TP2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TQ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TR2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TS2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TT2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TU2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TV2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TW2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TX2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TY2" t="s">
-        <v>137</v>
-      </c>
-      <c r="TZ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="UA2" t="s">
-        <v>137</v>
-      </c>
-      <c r="UB2" t="s">
-        <v>137</v>
-      </c>
-      <c r="UC2" t="s">
-        <v>652</v>
-      </c>
-      <c r="UD2" t="s">
-        <v>137</v>
-      </c>
-      <c r="UE2" t="s">
-        <v>609</v>
-      </c>
-      <c r="UF2" t="s">
-        <v>137</v>
-      </c>
-      <c r="UG2" t="s">
-        <v>652</v>
-      </c>
-      <c r="UH2" t="s">
-        <v>137</v>
-      </c>
-      <c r="UI2" t="s">
-        <v>609</v>
-      </c>
-      <c r="UJ2" t="s">
-        <v>137</v>
-      </c>
-      <c r="UK2" t="s">
-        <v>652</v>
-      </c>
-      <c r="UL2" t="s">
-        <v>137</v>
-      </c>
-      <c r="UM2" t="s">
-        <v>609</v>
-      </c>
-      <c r="UN2" t="s">
-        <v>137</v>
-      </c>
-      <c r="UO2" t="s">
-        <v>652</v>
-      </c>
       <c r="UP2" t="s">
         <v>137</v>
       </c>
       <c r="UQ2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>